<commit_message>
compiled with new full catalog paths to images
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="304">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1431,7 +1431,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="486">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1545,6 +1545,1275 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1854,12 +3123,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="29.71" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="27.29" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="8.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="25.71" collapsed="false"/>
-    <col min="6" max="26" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.71" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.29" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.71" collapsed="true"/>
+    <col min="6" max="26" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
@@ -9329,13 +10598,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.29" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.71" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="22.86" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="21.71" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="112.43" collapsed="false"/>
-    <col min="7" max="27" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.29" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.71" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.86" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.71" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="112.43" collapsed="true"/>
+    <col min="7" max="27" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -9390,162 +10659,162 @@
       <c r="AA2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="103" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="104" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="105" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="106" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="107" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="108" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="109" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="110" t="s">
         <v>40</v>
       </c>
     </row>
@@ -9587,17 +10856,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.71" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.43" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.43" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="8.43" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="28.43" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.43" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="8" max="9" customWidth="true" width="21.43" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="35.14" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="16.71" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="21.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="9.71" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.43" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.43" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.43" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.43" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.43" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="21.43" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="35.14" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.71" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="21.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -9673,25 +10942,25 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="138" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="156" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="165" t="s">
         <v>69</v>
       </c>
       <c r="J3"/>
@@ -9699,25 +10968,25 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="130" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="139" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="148" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="157" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="59" t="s">
+      <c r="I4" s="166" t="s">
         <v>74</v>
       </c>
       <c r="J4"/>
@@ -9725,25 +10994,25 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="122" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="131" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="140" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="149" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="158" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="167" t="s">
         <v>79</v>
       </c>
       <c r="J5"/>
@@ -9751,25 +11020,25 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="123" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="141" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="150" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="159" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="168" t="s">
         <v>83</v>
       </c>
       <c r="J6"/>
@@ -9777,25 +11046,25 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="124" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="133" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="142" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="151" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="160" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="169" t="s">
         <v>87</v>
       </c>
       <c r="J7"/>
@@ -9803,25 +11072,25 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="125" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="143" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="161" t="s">
         <v>90</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="170" t="s">
         <v>91</v>
       </c>
       <c r="J8"/>
@@ -9829,25 +11098,25 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="126" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="135" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="153" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="162" t="s">
         <v>94</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="171" t="s">
         <v>95</v>
       </c>
       <c r="J9"/>
@@ -9855,25 +11124,25 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="127" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="136" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="145" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="154" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="59" t="s">
+      <c r="H10" s="163" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="59" t="s">
+      <c r="I10" s="172" t="s">
         <v>99</v>
       </c>
       <c r="J10"/>
@@ -9881,25 +11150,25 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="137" t="s">
         <v>100</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="146" t="s">
         <v>101</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="155" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="164" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="173" t="s">
         <v>103</v>
       </c>
       <c r="J11"/>
@@ -10388,18 +11657,18 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.14" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="11.71" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.43" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="9.43" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="13.86" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.86" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="29.71" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="16.43" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="19.14" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="21.43" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="19.0" collapsed="false"/>
-    <col min="12" max="31" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.14" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.71" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.43" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.43" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.86" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.86" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.71" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.43" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.14" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.43" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="12" max="31" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -10495,31 +11764,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="174" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="195" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="216" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="234" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="255" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="276" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="297" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="318" t="s">
         <v>111</v>
       </c>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="339" t="s">
         <v>111</v>
       </c>
       <c r="U3" s="9"/>
@@ -10533,31 +11802,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="196" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="217" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="235" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="256" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="277" t="s">
         <v>114</v>
       </c>
-      <c r="I4" s="59" t="s">
+      <c r="I4" s="298" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="59" t="s">
+      <c r="J4" s="319" t="s">
         <v>115</v>
       </c>
-      <c r="K4" s="59" t="s">
+      <c r="K4" s="340" t="s">
         <v>115</v>
       </c>
       <c r="U4" s="9"/>
@@ -10571,31 +11840,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="197" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="218" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="236" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="257" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="278" t="s">
         <v>117</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="299" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="320" t="s">
         <v>118</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="341" t="s">
         <v>118</v>
       </c>
       <c r="U5" s="9"/>
@@ -10609,31 +11878,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="177" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="198" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="219" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="237" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="258" t="s">
         <v>119</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="279" t="s">
         <v>120</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="300" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="59" t="s">
+      <c r="J6" s="321" t="s">
         <v>121</v>
       </c>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="342" t="s">
         <v>121</v>
       </c>
       <c r="U6" s="9"/>
@@ -10647,31 +11916,31 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="178" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="199" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="220" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="238" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="259" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="280" t="s">
         <v>123</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="301" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="59" t="s">
+      <c r="J7" s="322" t="s">
         <v>124</v>
       </c>
-      <c r="K7" s="59" t="s">
+      <c r="K7" s="343" t="s">
         <v>124</v>
       </c>
       <c r="U7" s="9"/>
@@ -10685,31 +11954,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="179" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="200" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="221" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="239" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="260" t="s">
         <v>125</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="281" t="s">
         <v>126</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="302" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="323" t="s">
         <v>127</v>
       </c>
-      <c r="K8" s="59" t="s">
+      <c r="K8" s="344" t="s">
         <v>127</v>
       </c>
       <c r="U8" s="9"/>
@@ -10723,29 +11992,29 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="180" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="201" t="s">
         <v>75</v>
       </c>
       <c r="E9" s="24"/>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="240" t="s">
         <v>128</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="261" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="282" t="s">
         <v>130</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="303" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="324" t="s">
         <v>131</v>
       </c>
-      <c r="K9" s="59" t="s">
+      <c r="K9" s="345" t="s">
         <v>131</v>
       </c>
       <c r="U9" s="9"/>
@@ -10759,31 +12028,31 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="181" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="202" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="222" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="241" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="262" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="59" t="s">
+      <c r="H10" s="283" t="s">
         <v>133</v>
       </c>
-      <c r="I10" s="59" t="s">
+      <c r="I10" s="304" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="59" t="s">
+      <c r="J10" s="325" t="s">
         <v>134</v>
       </c>
-      <c r="K10" s="59" t="s">
+      <c r="K10" s="346" t="s">
         <v>134</v>
       </c>
       <c r="U10" s="9"/>
@@ -10797,31 +12066,31 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="182" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="203" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="223" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="242" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="263" t="s">
         <v>135</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="284" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="305" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="326" t="s">
         <v>137</v>
       </c>
-      <c r="K11" s="59" t="s">
+      <c r="K11" s="347" t="s">
         <v>137</v>
       </c>
       <c r="U11" s="9"/>
@@ -10835,31 +12104,31 @@
     <row r="12">
       <c r="A12" s="24"/>
       <c r="B12"/>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="183" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="59" t="s">
+      <c r="D12" s="204" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="224" t="s">
         <v>108</v>
       </c>
-      <c r="F12" s="59" t="s">
+      <c r="F12" s="243" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="264" t="s">
         <v>138</v>
       </c>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="285" t="s">
         <v>139</v>
       </c>
-      <c r="I12" s="59" t="s">
+      <c r="I12" s="306" t="s">
         <v>67</v>
       </c>
-      <c r="J12" s="59" t="s">
+      <c r="J12" s="327" t="s">
         <v>140</v>
       </c>
-      <c r="K12" s="59" t="s">
+      <c r="K12" s="348" t="s">
         <v>140</v>
       </c>
       <c r="U12" s="9"/>
@@ -10873,31 +12142,31 @@
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13"/>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="184" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="205" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="225" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="59" t="s">
+      <c r="F13" s="244" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="265" t="s">
         <v>141</v>
       </c>
-      <c r="H13" s="59" t="s">
+      <c r="H13" s="286" t="s">
         <v>142</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="307" t="s">
         <v>67</v>
       </c>
-      <c r="J13" s="59" t="s">
+      <c r="J13" s="328" t="s">
         <v>143</v>
       </c>
-      <c r="K13" s="59" t="s">
+      <c r="K13" s="349" t="s">
         <v>143</v>
       </c>
       <c r="U13" s="9"/>
@@ -10911,31 +12180,31 @@
     <row r="14">
       <c r="A14" s="24"/>
       <c r="B14"/>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="185" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="206" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="226" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="59" t="s">
+      <c r="F14" s="245" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="59" t="s">
+      <c r="G14" s="266" t="s">
         <v>144</v>
       </c>
-      <c r="H14" s="59" t="s">
+      <c r="H14" s="287" t="s">
         <v>145</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="308" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="59" t="s">
+      <c r="J14" s="329" t="s">
         <v>146</v>
       </c>
-      <c r="K14" s="59" t="s">
+      <c r="K14" s="350" t="s">
         <v>146</v>
       </c>
       <c r="U14" s="9"/>
@@ -10949,31 +12218,31 @@
     <row r="15">
       <c r="A15" s="24"/>
       <c r="B15"/>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="186" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="59" t="s">
+      <c r="D15" s="207" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="227" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F15" s="246" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="59" t="s">
+      <c r="G15" s="267" t="s">
         <v>147</v>
       </c>
-      <c r="H15" s="59" t="s">
+      <c r="H15" s="288" t="s">
         <v>148</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I15" s="309" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="59" t="s">
+      <c r="J15" s="330" t="s">
         <v>149</v>
       </c>
-      <c r="K15" s="59" t="s">
+      <c r="K15" s="351" t="s">
         <v>149</v>
       </c>
       <c r="U15" s="9"/>
@@ -10987,29 +12256,29 @@
     <row r="16">
       <c r="A16" s="24"/>
       <c r="B16"/>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="187" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="208" t="s">
         <v>75</v>
       </c>
       <c r="E16" s="24"/>
-      <c r="F16" s="59" t="s">
+      <c r="F16" s="247" t="s">
         <v>128</v>
       </c>
-      <c r="G16" s="59" t="s">
+      <c r="G16" s="268" t="s">
         <v>150</v>
       </c>
-      <c r="H16" s="59" t="s">
+      <c r="H16" s="289" t="s">
         <v>151</v>
       </c>
-      <c r="I16" s="59" t="s">
+      <c r="I16" s="310" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="59" t="s">
+      <c r="J16" s="331" t="s">
         <v>152</v>
       </c>
-      <c r="K16" s="59" t="s">
+      <c r="K16" s="352" t="s">
         <v>152</v>
       </c>
       <c r="U16" s="9"/>
@@ -11023,31 +12292,31 @@
     <row r="17">
       <c r="A17" s="24"/>
       <c r="B17"/>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="188" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D17" s="209" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="59" t="s">
+      <c r="E17" s="228" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="59" t="s">
+      <c r="F17" s="248" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="59" t="s">
+      <c r="G17" s="269" t="s">
         <v>153</v>
       </c>
-      <c r="H17" s="59" t="s">
+      <c r="H17" s="290" t="s">
         <v>154</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="I17" s="311" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="59" t="s">
+      <c r="J17" s="332" t="s">
         <v>155</v>
       </c>
-      <c r="K17" s="59" t="s">
+      <c r="K17" s="353" t="s">
         <v>155</v>
       </c>
       <c r="U17" s="9"/>
@@ -11061,31 +12330,31 @@
     <row r="18">
       <c r="A18" s="24"/>
       <c r="B18"/>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="189" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="210" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="229" t="s">
         <v>112</v>
       </c>
-      <c r="F18" s="59" t="s">
+      <c r="F18" s="249" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="59" t="s">
+      <c r="G18" s="270" t="s">
         <v>156</v>
       </c>
-      <c r="H18" s="59" t="s">
+      <c r="H18" s="291" t="s">
         <v>157</v>
       </c>
-      <c r="I18" s="59" t="s">
+      <c r="I18" s="312" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="59" t="s">
+      <c r="J18" s="333" t="s">
         <v>158</v>
       </c>
-      <c r="K18" s="59" t="s">
+      <c r="K18" s="354" t="s">
         <v>158</v>
       </c>
       <c r="U18" s="9"/>
@@ -11099,31 +12368,31 @@
     <row r="19">
       <c r="A19" s="24"/>
       <c r="B19"/>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="190" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="59" t="s">
+      <c r="D19" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="59" t="s">
+      <c r="E19" s="230" t="s">
         <v>108</v>
       </c>
-      <c r="F19" s="59" t="s">
+      <c r="F19" s="250" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="59" t="s">
+      <c r="G19" s="271" t="s">
         <v>159</v>
       </c>
-      <c r="H19" s="59" t="s">
+      <c r="H19" s="292" t="s">
         <v>160</v>
       </c>
-      <c r="I19" s="59" t="s">
+      <c r="I19" s="313" t="s">
         <v>67</v>
       </c>
-      <c r="J19" s="59" t="s">
+      <c r="J19" s="334" t="s">
         <v>161</v>
       </c>
-      <c r="K19" s="59" t="s">
+      <c r="K19" s="355" t="s">
         <v>161</v>
       </c>
       <c r="U19" s="9"/>
@@ -11137,31 +12406,31 @@
     <row r="20">
       <c r="A20" s="24"/>
       <c r="B20"/>
-      <c r="C20" s="59" t="s">
+      <c r="C20" s="191" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="212" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="59" t="s">
+      <c r="E20" s="231" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="59" t="s">
+      <c r="F20" s="251" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="59" t="s">
+      <c r="G20" s="272" t="s">
         <v>162</v>
       </c>
-      <c r="H20" s="59" t="s">
+      <c r="H20" s="293" t="s">
         <v>163</v>
       </c>
-      <c r="I20" s="59" t="s">
+      <c r="I20" s="314" t="s">
         <v>67</v>
       </c>
-      <c r="J20" s="59" t="s">
+      <c r="J20" s="335" t="s">
         <v>164</v>
       </c>
-      <c r="K20" s="59" t="s">
+      <c r="K20" s="356" t="s">
         <v>164</v>
       </c>
       <c r="U20" s="9"/>
@@ -11175,31 +12444,31 @@
     <row r="21">
       <c r="A21" s="24"/>
       <c r="B21"/>
-      <c r="C21" s="59" t="s">
+      <c r="C21" s="192" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="59" t="s">
+      <c r="D21" s="213" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="E21" s="232" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="59" t="s">
+      <c r="F21" s="252" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="59" t="s">
+      <c r="G21" s="273" t="s">
         <v>165</v>
       </c>
-      <c r="H21" s="59" t="s">
+      <c r="H21" s="294" t="s">
         <v>166</v>
       </c>
-      <c r="I21" s="59" t="s">
+      <c r="I21" s="315" t="s">
         <v>67</v>
       </c>
-      <c r="J21" s="59" t="s">
+      <c r="J21" s="336" t="s">
         <v>167</v>
       </c>
-      <c r="K21" s="59" t="s">
+      <c r="K21" s="357" t="s">
         <v>167</v>
       </c>
       <c r="U21" s="9"/>
@@ -11213,31 +12482,31 @@
     <row r="22">
       <c r="A22" s="24"/>
       <c r="B22"/>
-      <c r="C22" s="59" t="s">
+      <c r="C22" s="193" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="214" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="59" t="s">
+      <c r="E22" s="233" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="59" t="s">
+      <c r="F22" s="253" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="59" t="s">
+      <c r="G22" s="274" t="s">
         <v>168</v>
       </c>
-      <c r="H22" s="59" t="s">
+      <c r="H22" s="295" t="s">
         <v>169</v>
       </c>
-      <c r="I22" s="59" t="s">
+      <c r="I22" s="316" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="337" t="s">
         <v>170</v>
       </c>
-      <c r="K22" s="59" t="s">
+      <c r="K22" s="358" t="s">
         <v>170</v>
       </c>
       <c r="U22" s="9"/>
@@ -11251,29 +12520,29 @@
     <row r="23">
       <c r="A23" s="24"/>
       <c r="B23"/>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="59" t="s">
+      <c r="D23" s="215" t="s">
         <v>75</v>
       </c>
       <c r="E23" s="24"/>
-      <c r="F23" s="59" t="s">
+      <c r="F23" s="254" t="s">
         <v>128</v>
       </c>
-      <c r="G23" s="59" t="s">
+      <c r="G23" s="275" t="s">
         <v>171</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="296" t="s">
         <v>172</v>
       </c>
-      <c r="I23" s="59" t="s">
+      <c r="I23" s="317" t="s">
         <v>67</v>
       </c>
-      <c r="J23" s="59" t="s">
+      <c r="J23" s="338" t="s">
         <v>173</v>
       </c>
-      <c r="K23" s="59" t="s">
+      <c r="K23" s="359" t="s">
         <v>173</v>
       </c>
       <c r="U23" s="9"/>
@@ -12167,19 +13436,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.29" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.86" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.43" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="7.14" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="19.43" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.71" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.43" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="19.29" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.14" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="21.86" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="28.14" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="16.71" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="21.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.29" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.86" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.43" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="7.14" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.43" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.71" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.43" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.29" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.14" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.86" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.14" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.71" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="21.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.75" customHeight="1">
@@ -12259,28 +13528,28 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="360" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="369" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="378" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="387" t="s">
         <v>178</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="396" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="405" t="s">
         <v>179</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="414" t="s">
         <v>180</v>
       </c>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="423" t="s">
         <v>181</v>
       </c>
       <c r="K3"/>
@@ -12288,28 +13557,28 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="361" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="370" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="379" t="s">
         <v>182</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="388" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="397" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="406" t="s">
         <v>184</v>
       </c>
-      <c r="I4" s="59" t="s">
+      <c r="I4" s="415" t="s">
         <v>185</v>
       </c>
-      <c r="J4" s="59" t="s">
+      <c r="J4" s="424" t="s">
         <v>186</v>
       </c>
       <c r="K4"/>
@@ -12317,28 +13586,28 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="362" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="371" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="380" t="s">
         <v>187</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="389" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="398" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="407" t="s">
         <v>189</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="416" t="s">
         <v>190</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="425" t="s">
         <v>191</v>
       </c>
       <c r="K5"/>
@@ -12346,28 +13615,28 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="363" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="372" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="381" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="390" t="s">
         <v>193</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="399" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="408" t="s">
         <v>194</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="417" t="s">
         <v>195</v>
       </c>
-      <c r="J6" s="59" t="s">
+      <c r="J6" s="426" t="s">
         <v>196</v>
       </c>
       <c r="K6"/>
@@ -12375,28 +13644,28 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="364" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="373" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="382" t="s">
         <v>197</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="391" t="s">
         <v>198</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="400" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="409" t="s">
         <v>199</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="418" t="s">
         <v>200</v>
       </c>
-      <c r="J7" s="59" t="s">
+      <c r="J7" s="427" t="s">
         <v>201</v>
       </c>
       <c r="K7"/>
@@ -12404,28 +13673,28 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="365" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="374" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="383" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="392" t="s">
         <v>203</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="401" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="410" t="s">
         <v>204</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="419" t="s">
         <v>205</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="428" t="s">
         <v>206</v>
       </c>
       <c r="K8"/>
@@ -12433,28 +13702,28 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="366" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="375" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="384" t="s">
         <v>207</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="393" t="s">
         <v>208</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="402" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="411" t="s">
         <v>209</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="420" t="s">
         <v>210</v>
       </c>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="429" t="s">
         <v>211</v>
       </c>
       <c r="K9"/>
@@ -12462,28 +13731,28 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="367" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="376" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="385" t="s">
         <v>212</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="394" t="s">
         <v>213</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="403" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="59" t="s">
+      <c r="H10" s="412" t="s">
         <v>214</v>
       </c>
-      <c r="I10" s="59" t="s">
+      <c r="I10" s="421" t="s">
         <v>215</v>
       </c>
-      <c r="J10" s="59" t="s">
+      <c r="J10" s="430" t="s">
         <v>216</v>
       </c>
       <c r="K10"/>
@@ -12491,28 +13760,28 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="368" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="377" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="386" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="395" t="s">
         <v>218</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="404" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="413" t="s">
         <v>219</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="422" t="s">
         <v>220</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="431" t="s">
         <v>221</v>
       </c>
       <c r="K11"/>
@@ -13111,19 +14380,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="7.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="8.29" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.29" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="9.43" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="10.29" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="39.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="22.43" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="17.43" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.43" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="16.43" collapsed="false"/>
-    <col min="12" max="13" customWidth="true" width="10.86" collapsed="false"/>
-    <col min="14" max="31" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.29" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.29" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.43" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.29" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.43" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.43" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.43" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.43" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="10.86" collapsed="true"/>
+    <col min="14" max="31" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -13199,31 +14468,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="432" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="438" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="444" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="450" t="s">
         <v>224</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="456" t="s">
         <v>225</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="462" t="s">
         <v>226</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="468" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="474" t="s">
         <v>227</v>
       </c>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="480" t="s">
         <v>228</v>
       </c>
       <c r="U3" s="9"/>
@@ -13239,31 +14508,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="433" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="439" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="445" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="451" t="s">
         <v>229</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="457" t="s">
         <v>230</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="463" t="s">
         <v>231</v>
       </c>
-      <c r="I4" s="59" t="s">
+      <c r="I4" s="469" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="59" t="s">
+      <c r="J4" s="475" t="s">
         <v>232</v>
       </c>
-      <c r="K4" s="59" t="s">
+      <c r="K4" s="481" t="s">
         <v>233</v>
       </c>
       <c r="U4" s="9"/>
@@ -13279,31 +14548,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="434" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="440" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="446" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="452" t="s">
         <v>224</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="458" t="s">
         <v>234</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="464" t="s">
         <v>235</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="470" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="476" t="s">
         <v>236</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="482" t="s">
         <v>228</v>
       </c>
       <c r="U5" s="9"/>
@@ -13319,31 +14588,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="435" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="441" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="447" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="453" t="s">
         <v>229</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="459" t="s">
         <v>230</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="465" t="s">
         <v>237</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="471" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="59" t="s">
+      <c r="J6" s="477" t="s">
         <v>238</v>
       </c>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="483" t="s">
         <v>233</v>
       </c>
       <c r="U6" s="9"/>
@@ -13359,31 +14628,31 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="436" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="442" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="448" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="454" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="460" t="s">
         <v>239</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="466" t="s">
         <v>240</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="472" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="59" t="s">
+      <c r="J7" s="478" t="s">
         <v>241</v>
       </c>
-      <c r="K7" s="59" t="s">
+      <c r="K7" s="484" t="s">
         <v>242</v>
       </c>
       <c r="U7" s="9"/>
@@ -13399,31 +14668,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="437" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="443" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="449" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="455" t="s">
         <v>229</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="461" t="s">
         <v>230</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="467" t="s">
         <v>243</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="473" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="479" t="s">
         <v>244</v>
       </c>
-      <c r="K8" s="59" t="s">
+      <c r="K8" s="485" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="9"/>
@@ -14681,16 +15950,16 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="8.29" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="10.29" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.57" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="15.43" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="57.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="22.71" collapsed="false"/>
-    <col min="7" max="8" customWidth="true" width="14.29" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="20.43" collapsed="false"/>
-    <col min="10" max="12" customWidth="true" width="15.14" collapsed="false"/>
-    <col min="13" max="14" customWidth="true" width="16.29" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="8.29" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.29" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.57" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.43" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="57.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.71" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="14.29" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.43" collapsed="true"/>
+    <col min="10" max="12" customWidth="true" width="15.14" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="16.29" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
@@ -23325,8 +24594,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="150.0" collapsed="false"/>
-    <col min="2" max="6" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="150.0" collapsed="true"/>
+    <col min="2" max="6" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-03-03 23:32:14]  updating research background
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9919" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10342" uniqueCount="304">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1431,7 +1431,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8946">
+  <cellXfs count="9369">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1545,6 +1545,1275 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -36039,162 +37308,162 @@
       <c r="AA2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="8523" t="s">
+      <c r="A3" s="8946" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8531" t="s">
+      <c r="B3" s="8954" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="8539" t="s">
+      <c r="C3" s="8962" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="8547" t="s">
+      <c r="D3" s="8970" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="8555" t="s">
+      <c r="E3" s="8978" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="8563" t="s">
+      <c r="F3" s="8986" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8524" t="s">
+      <c r="A4" s="8947" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8532" t="s">
+      <c r="B4" s="8955" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="8540" t="s">
+      <c r="C4" s="8963" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="8548" t="s">
+      <c r="D4" s="8971" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="8556" t="s">
+      <c r="E4" s="8979" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="8564" t="s">
+      <c r="F4" s="8987" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8525" t="s">
+      <c r="A5" s="8948" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8533" t="s">
+      <c r="B5" s="8956" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="8541" t="s">
+      <c r="C5" s="8964" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="8549" t="s">
+      <c r="D5" s="8972" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="8557" t="s">
+      <c r="E5" s="8980" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="8565" t="s">
+      <c r="F5" s="8988" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8526" t="s">
+      <c r="A6" s="8949" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8534" t="s">
+      <c r="B6" s="8957" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="8542" t="s">
+      <c r="C6" s="8965" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="8550" t="s">
+      <c r="D6" s="8973" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="8558" t="s">
+      <c r="E6" s="8981" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="8566" t="s">
+      <c r="F6" s="8989" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8527" t="s">
+      <c r="A7" s="8950" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8535" t="s">
+      <c r="B7" s="8958" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="8543" t="s">
+      <c r="C7" s="8966" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="8551" t="s">
+      <c r="D7" s="8974" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="8559" t="s">
+      <c r="E7" s="8982" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="8567" t="s">
+      <c r="F7" s="8990" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8528" t="s">
+      <c r="A8" s="8951" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="8536" t="s">
+      <c r="B8" s="8959" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="8544" t="s">
+      <c r="C8" s="8967" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="8552" t="s">
+      <c r="D8" s="8975" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="8560" t="s">
+      <c r="E8" s="8983" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="8568" t="s">
+      <c r="F8" s="8991" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8529" t="s">
+      <c r="A9" s="8952" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="8537" t="s">
+      <c r="B9" s="8960" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="8545" t="s">
+      <c r="C9" s="8968" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="8553" t="s">
+      <c r="D9" s="8976" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="8561" t="s">
+      <c r="E9" s="8984" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="8569" t="s">
+      <c r="F9" s="8992" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8530" t="s">
+      <c r="A10" s="8953" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="8538" t="s">
+      <c r="B10" s="8961" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="8546" t="s">
+      <c r="C10" s="8969" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="8554" t="s">
+      <c r="D10" s="8977" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="8562" t="s">
+      <c r="E10" s="8985" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="8570" t="s">
+      <c r="F10" s="8993" t="s">
         <v>40</v>
       </c>
     </row>
@@ -36322,25 +37591,25 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="8571" t="s">
+      <c r="C3" s="8994" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="8580" t="s">
+      <c r="D3" s="9003" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="8589" t="s">
+      <c r="E3" s="9012" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="8598" t="s">
+      <c r="F3" s="9021" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="8607" t="s">
+      <c r="G3" s="9030" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="8616" t="s">
+      <c r="H3" s="9039" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="8625" t="s">
+      <c r="I3" s="9048" t="s">
         <v>69</v>
       </c>
       <c r="J3"/>
@@ -36348,25 +37617,25 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="8572" t="s">
+      <c r="C4" s="8995" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="8581" t="s">
+      <c r="D4" s="9004" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="8590" t="s">
+      <c r="E4" s="9013" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="8599" t="s">
+      <c r="F4" s="9022" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="8608" t="s">
+      <c r="G4" s="9031" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="8617" t="s">
+      <c r="H4" s="9040" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="8626" t="s">
+      <c r="I4" s="9049" t="s">
         <v>74</v>
       </c>
       <c r="J4"/>
@@ -36374,25 +37643,25 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="8573" t="s">
+      <c r="C5" s="8996" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="8582" t="s">
+      <c r="D5" s="9005" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="8591" t="s">
+      <c r="E5" s="9014" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="8600" t="s">
+      <c r="F5" s="9023" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="8609" t="s">
+      <c r="G5" s="9032" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="8618" t="s">
+      <c r="H5" s="9041" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="8627" t="s">
+      <c r="I5" s="9050" t="s">
         <v>79</v>
       </c>
       <c r="J5"/>
@@ -36400,25 +37669,25 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="8574" t="s">
+      <c r="C6" s="8997" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="8583" t="s">
+      <c r="D6" s="9006" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="8592" t="s">
+      <c r="E6" s="9015" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="8601" t="s">
+      <c r="F6" s="9024" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="8610" t="s">
+      <c r="G6" s="9033" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="8619" t="s">
+      <c r="H6" s="9042" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="8628" t="s">
+      <c r="I6" s="9051" t="s">
         <v>83</v>
       </c>
       <c r="J6"/>
@@ -36426,25 +37695,25 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="8575" t="s">
+      <c r="C7" s="8998" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="8584" t="s">
+      <c r="D7" s="9007" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="8593" t="s">
+      <c r="E7" s="9016" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="8602" t="s">
+      <c r="F7" s="9025" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="8611" t="s">
+      <c r="G7" s="9034" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="8620" t="s">
+      <c r="H7" s="9043" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="8629" t="s">
+      <c r="I7" s="9052" t="s">
         <v>87</v>
       </c>
       <c r="J7"/>
@@ -36452,25 +37721,25 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="8576" t="s">
+      <c r="C8" s="8999" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="8585" t="s">
+      <c r="D8" s="9008" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="8594" t="s">
+      <c r="E8" s="9017" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="8603" t="s">
+      <c r="F8" s="9026" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="8612" t="s">
+      <c r="G8" s="9035" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="8621" t="s">
+      <c r="H8" s="9044" t="s">
         <v>90</v>
       </c>
-      <c r="I8" s="8630" t="s">
+      <c r="I8" s="9053" t="s">
         <v>91</v>
       </c>
       <c r="J8"/>
@@ -36478,25 +37747,25 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="8577" t="s">
+      <c r="C9" s="9000" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="8586" t="s">
+      <c r="D9" s="9009" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="8595" t="s">
+      <c r="E9" s="9018" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="8604" t="s">
+      <c r="F9" s="9027" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="8613" t="s">
+      <c r="G9" s="9036" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="8622" t="s">
+      <c r="H9" s="9045" t="s">
         <v>94</v>
       </c>
-      <c r="I9" s="8631" t="s">
+      <c r="I9" s="9054" t="s">
         <v>95</v>
       </c>
       <c r="J9"/>
@@ -36504,25 +37773,25 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="8578" t="s">
+      <c r="C10" s="9001" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="8587" t="s">
+      <c r="D10" s="9010" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="8596" t="s">
+      <c r="E10" s="9019" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="8605" t="s">
+      <c r="F10" s="9028" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="8614" t="s">
+      <c r="G10" s="9037" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="8623" t="s">
+      <c r="H10" s="9046" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="8632" t="s">
+      <c r="I10" s="9055" t="s">
         <v>99</v>
       </c>
       <c r="J10"/>
@@ -36530,25 +37799,25 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="8579" t="s">
+      <c r="C11" s="9002" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="8588" t="s">
+      <c r="D11" s="9011" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="8597" t="s">
+      <c r="E11" s="9020" t="s">
         <v>100</v>
       </c>
-      <c r="F11" s="8606" t="s">
+      <c r="F11" s="9029" t="s">
         <v>101</v>
       </c>
-      <c r="G11" s="8615" t="s">
+      <c r="G11" s="9038" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="8624" t="s">
+      <c r="H11" s="9047" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="8633" t="s">
+      <c r="I11" s="9056" t="s">
         <v>103</v>
       </c>
       <c r="J11"/>
@@ -37144,31 +38413,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="8634" t="s">
+      <c r="C3" s="9057" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="8655" t="s">
+      <c r="D3" s="9078" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="8676" t="s">
+      <c r="E3" s="9099" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="8694" t="s">
+      <c r="F3" s="9117" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="8715" t="s">
+      <c r="G3" s="9138" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="8736" t="s">
+      <c r="H3" s="9159" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="8757" t="s">
+      <c r="I3" s="9180" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="8778" t="s">
+      <c r="J3" s="9201" t="s">
         <v>111</v>
       </c>
-      <c r="K3" s="8799" t="s">
+      <c r="K3" s="9222" t="s">
         <v>111</v>
       </c>
       <c r="U3" s="9"/>
@@ -37182,31 +38451,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="8635" t="s">
+      <c r="C4" s="9058" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="8656" t="s">
+      <c r="D4" s="9079" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="8677" t="s">
+      <c r="E4" s="9100" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="8695" t="s">
+      <c r="F4" s="9118" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="8716" t="s">
+      <c r="G4" s="9139" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="8737" t="s">
+      <c r="H4" s="9160" t="s">
         <v>114</v>
       </c>
-      <c r="I4" s="8758" t="s">
+      <c r="I4" s="9181" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="8779" t="s">
+      <c r="J4" s="9202" t="s">
         <v>115</v>
       </c>
-      <c r="K4" s="8800" t="s">
+      <c r="K4" s="9223" t="s">
         <v>115</v>
       </c>
       <c r="U4" s="9"/>
@@ -37220,31 +38489,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="8636" t="s">
+      <c r="C5" s="9059" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="8657" t="s">
+      <c r="D5" s="9080" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="8678" t="s">
+      <c r="E5" s="9101" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="8696" t="s">
+      <c r="F5" s="9119" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="8717" t="s">
+      <c r="G5" s="9140" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="8738" t="s">
+      <c r="H5" s="9161" t="s">
         <v>117</v>
       </c>
-      <c r="I5" s="8759" t="s">
+      <c r="I5" s="9182" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="8780" t="s">
+      <c r="J5" s="9203" t="s">
         <v>118</v>
       </c>
-      <c r="K5" s="8801" t="s">
+      <c r="K5" s="9224" t="s">
         <v>118</v>
       </c>
       <c r="U5" s="9"/>
@@ -37258,31 +38527,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="8637" t="s">
+      <c r="C6" s="9060" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="8658" t="s">
+      <c r="D6" s="9081" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="8679" t="s">
+      <c r="E6" s="9102" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="8697" t="s">
+      <c r="F6" s="9120" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="8718" t="s">
+      <c r="G6" s="9141" t="s">
         <v>119</v>
       </c>
-      <c r="H6" s="8739" t="s">
+      <c r="H6" s="9162" t="s">
         <v>120</v>
       </c>
-      <c r="I6" s="8760" t="s">
+      <c r="I6" s="9183" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="8781" t="s">
+      <c r="J6" s="9204" t="s">
         <v>121</v>
       </c>
-      <c r="K6" s="8802" t="s">
+      <c r="K6" s="9225" t="s">
         <v>121</v>
       </c>
       <c r="U6" s="9"/>
@@ -37296,31 +38565,31 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="8638" t="s">
+      <c r="C7" s="9061" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="8659" t="s">
+      <c r="D7" s="9082" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="8680" t="s">
+      <c r="E7" s="9103" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="8698" t="s">
+      <c r="F7" s="9121" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8719" t="s">
+      <c r="G7" s="9142" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="8740" t="s">
+      <c r="H7" s="9163" t="s">
         <v>123</v>
       </c>
-      <c r="I7" s="8761" t="s">
+      <c r="I7" s="9184" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="8782" t="s">
+      <c r="J7" s="9205" t="s">
         <v>124</v>
       </c>
-      <c r="K7" s="8803" t="s">
+      <c r="K7" s="9226" t="s">
         <v>124</v>
       </c>
       <c r="U7" s="9"/>
@@ -37334,31 +38603,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="8639" t="s">
+      <c r="C8" s="9062" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="8660" t="s">
+      <c r="D8" s="9083" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="8681" t="s">
+      <c r="E8" s="9104" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="8699" t="s">
+      <c r="F8" s="9122" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="8720" t="s">
+      <c r="G8" s="9143" t="s">
         <v>125</v>
       </c>
-      <c r="H8" s="8741" t="s">
+      <c r="H8" s="9164" t="s">
         <v>126</v>
       </c>
-      <c r="I8" s="8762" t="s">
+      <c r="I8" s="9185" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="8783" t="s">
+      <c r="J8" s="9206" t="s">
         <v>127</v>
       </c>
-      <c r="K8" s="8804" t="s">
+      <c r="K8" s="9227" t="s">
         <v>127</v>
       </c>
       <c r="U8" s="9"/>
@@ -37372,29 +38641,29 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="8640" t="s">
+      <c r="C9" s="9063" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="8661" t="s">
+      <c r="D9" s="9084" t="s">
         <v>75</v>
       </c>
       <c r="E9" s="24"/>
-      <c r="F9" s="8700" t="s">
+      <c r="F9" s="9123" t="s">
         <v>128</v>
       </c>
-      <c r="G9" s="8721" t="s">
+      <c r="G9" s="9144" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="8742" t="s">
+      <c r="H9" s="9165" t="s">
         <v>130</v>
       </c>
-      <c r="I9" s="8763" t="s">
+      <c r="I9" s="9186" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="8784" t="s">
+      <c r="J9" s="9207" t="s">
         <v>131</v>
       </c>
-      <c r="K9" s="8805" t="s">
+      <c r="K9" s="9228" t="s">
         <v>131</v>
       </c>
       <c r="U9" s="9"/>
@@ -37408,31 +38677,31 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="8641" t="s">
+      <c r="C10" s="9064" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="8662" t="s">
+      <c r="D10" s="9085" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="8682" t="s">
+      <c r="E10" s="9105" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="8701" t="s">
+      <c r="F10" s="9124" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="8722" t="s">
+      <c r="G10" s="9145" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="8743" t="s">
+      <c r="H10" s="9166" t="s">
         <v>133</v>
       </c>
-      <c r="I10" s="8764" t="s">
+      <c r="I10" s="9187" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="8785" t="s">
+      <c r="J10" s="9208" t="s">
         <v>134</v>
       </c>
-      <c r="K10" s="8806" t="s">
+      <c r="K10" s="9229" t="s">
         <v>134</v>
       </c>
       <c r="U10" s="9"/>
@@ -37446,31 +38715,31 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="8642" t="s">
+      <c r="C11" s="9065" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="8663" t="s">
+      <c r="D11" s="9086" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="8683" t="s">
+      <c r="E11" s="9106" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="8702" t="s">
+      <c r="F11" s="9125" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="8723" t="s">
+      <c r="G11" s="9146" t="s">
         <v>135</v>
       </c>
-      <c r="H11" s="8744" t="s">
+      <c r="H11" s="9167" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="8765" t="s">
+      <c r="I11" s="9188" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="8786" t="s">
+      <c r="J11" s="9209" t="s">
         <v>137</v>
       </c>
-      <c r="K11" s="8807" t="s">
+      <c r="K11" s="9230" t="s">
         <v>137</v>
       </c>
       <c r="U11" s="9"/>
@@ -37484,31 +38753,31 @@
     <row r="12">
       <c r="A12" s="24"/>
       <c r="B12"/>
-      <c r="C12" s="8643" t="s">
+      <c r="C12" s="9066" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="8664" t="s">
+      <c r="D12" s="9087" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="8684" t="s">
+      <c r="E12" s="9107" t="s">
         <v>108</v>
       </c>
-      <c r="F12" s="8703" t="s">
+      <c r="F12" s="9126" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="8724" t="s">
+      <c r="G12" s="9147" t="s">
         <v>138</v>
       </c>
-      <c r="H12" s="8745" t="s">
+      <c r="H12" s="9168" t="s">
         <v>139</v>
       </c>
-      <c r="I12" s="8766" t="s">
+      <c r="I12" s="9189" t="s">
         <v>67</v>
       </c>
-      <c r="J12" s="8787" t="s">
+      <c r="J12" s="9210" t="s">
         <v>140</v>
       </c>
-      <c r="K12" s="8808" t="s">
+      <c r="K12" s="9231" t="s">
         <v>140</v>
       </c>
       <c r="U12" s="9"/>
@@ -37522,31 +38791,31 @@
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13"/>
-      <c r="C13" s="8644" t="s">
+      <c r="C13" s="9067" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="8665" t="s">
+      <c r="D13" s="9088" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="8685" t="s">
+      <c r="E13" s="9108" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="8704" t="s">
+      <c r="F13" s="9127" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="8725" t="s">
+      <c r="G13" s="9148" t="s">
         <v>141</v>
       </c>
-      <c r="H13" s="8746" t="s">
+      <c r="H13" s="9169" t="s">
         <v>142</v>
       </c>
-      <c r="I13" s="8767" t="s">
+      <c r="I13" s="9190" t="s">
         <v>67</v>
       </c>
-      <c r="J13" s="8788" t="s">
+      <c r="J13" s="9211" t="s">
         <v>143</v>
       </c>
-      <c r="K13" s="8809" t="s">
+      <c r="K13" s="9232" t="s">
         <v>143</v>
       </c>
       <c r="U13" s="9"/>
@@ -37560,31 +38829,31 @@
     <row r="14">
       <c r="A14" s="24"/>
       <c r="B14"/>
-      <c r="C14" s="8645" t="s">
+      <c r="C14" s="9068" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="8666" t="s">
+      <c r="D14" s="9089" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="8686" t="s">
+      <c r="E14" s="9109" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="8705" t="s">
+      <c r="F14" s="9128" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="8726" t="s">
+      <c r="G14" s="9149" t="s">
         <v>144</v>
       </c>
-      <c r="H14" s="8747" t="s">
+      <c r="H14" s="9170" t="s">
         <v>145</v>
       </c>
-      <c r="I14" s="8768" t="s">
+      <c r="I14" s="9191" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="8789" t="s">
+      <c r="J14" s="9212" t="s">
         <v>146</v>
       </c>
-      <c r="K14" s="8810" t="s">
+      <c r="K14" s="9233" t="s">
         <v>146</v>
       </c>
       <c r="U14" s="9"/>
@@ -37598,31 +38867,31 @@
     <row r="15">
       <c r="A15" s="24"/>
       <c r="B15"/>
-      <c r="C15" s="8646" t="s">
+      <c r="C15" s="9069" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="8667" t="s">
+      <c r="D15" s="9090" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="8687" t="s">
+      <c r="E15" s="9110" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="8706" t="s">
+      <c r="F15" s="9129" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="8727" t="s">
+      <c r="G15" s="9150" t="s">
         <v>147</v>
       </c>
-      <c r="H15" s="8748" t="s">
+      <c r="H15" s="9171" t="s">
         <v>148</v>
       </c>
-      <c r="I15" s="8769" t="s">
+      <c r="I15" s="9192" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="8790" t="s">
+      <c r="J15" s="9213" t="s">
         <v>149</v>
       </c>
-      <c r="K15" s="8811" t="s">
+      <c r="K15" s="9234" t="s">
         <v>149</v>
       </c>
       <c r="U15" s="9"/>
@@ -37636,29 +38905,29 @@
     <row r="16">
       <c r="A16" s="24"/>
       <c r="B16"/>
-      <c r="C16" s="8647" t="s">
+      <c r="C16" s="9070" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="8668" t="s">
+      <c r="D16" s="9091" t="s">
         <v>75</v>
       </c>
       <c r="E16" s="24"/>
-      <c r="F16" s="8707" t="s">
+      <c r="F16" s="9130" t="s">
         <v>128</v>
       </c>
-      <c r="G16" s="8728" t="s">
+      <c r="G16" s="9151" t="s">
         <v>150</v>
       </c>
-      <c r="H16" s="8749" t="s">
+      <c r="H16" s="9172" t="s">
         <v>151</v>
       </c>
-      <c r="I16" s="8770" t="s">
+      <c r="I16" s="9193" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="8791" t="s">
+      <c r="J16" s="9214" t="s">
         <v>152</v>
       </c>
-      <c r="K16" s="8812" t="s">
+      <c r="K16" s="9235" t="s">
         <v>152</v>
       </c>
       <c r="U16" s="9"/>
@@ -37672,31 +38941,31 @@
     <row r="17">
       <c r="A17" s="24"/>
       <c r="B17"/>
-      <c r="C17" s="8648" t="s">
+      <c r="C17" s="9071" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="8669" t="s">
+      <c r="D17" s="9092" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="8688" t="s">
+      <c r="E17" s="9111" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="8708" t="s">
+      <c r="F17" s="9131" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="8729" t="s">
+      <c r="G17" s="9152" t="s">
         <v>153</v>
       </c>
-      <c r="H17" s="8750" t="s">
+      <c r="H17" s="9173" t="s">
         <v>154</v>
       </c>
-      <c r="I17" s="8771" t="s">
+      <c r="I17" s="9194" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="8792" t="s">
+      <c r="J17" s="9215" t="s">
         <v>155</v>
       </c>
-      <c r="K17" s="8813" t="s">
+      <c r="K17" s="9236" t="s">
         <v>155</v>
       </c>
       <c r="U17" s="9"/>
@@ -37710,31 +38979,31 @@
     <row r="18">
       <c r="A18" s="24"/>
       <c r="B18"/>
-      <c r="C18" s="8649" t="s">
+      <c r="C18" s="9072" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="8670" t="s">
+      <c r="D18" s="9093" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="8689" t="s">
+      <c r="E18" s="9112" t="s">
         <v>112</v>
       </c>
-      <c r="F18" s="8709" t="s">
+      <c r="F18" s="9132" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="8730" t="s">
+      <c r="G18" s="9153" t="s">
         <v>156</v>
       </c>
-      <c r="H18" s="8751" t="s">
+      <c r="H18" s="9174" t="s">
         <v>157</v>
       </c>
-      <c r="I18" s="8772" t="s">
+      <c r="I18" s="9195" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="8793" t="s">
+      <c r="J18" s="9216" t="s">
         <v>158</v>
       </c>
-      <c r="K18" s="8814" t="s">
+      <c r="K18" s="9237" t="s">
         <v>158</v>
       </c>
       <c r="U18" s="9"/>
@@ -37748,31 +39017,31 @@
     <row r="19">
       <c r="A19" s="24"/>
       <c r="B19"/>
-      <c r="C19" s="8650" t="s">
+      <c r="C19" s="9073" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="8671" t="s">
+      <c r="D19" s="9094" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="8690" t="s">
+      <c r="E19" s="9113" t="s">
         <v>108</v>
       </c>
-      <c r="F19" s="8710" t="s">
+      <c r="F19" s="9133" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="8731" t="s">
+      <c r="G19" s="9154" t="s">
         <v>159</v>
       </c>
-      <c r="H19" s="8752" t="s">
+      <c r="H19" s="9175" t="s">
         <v>160</v>
       </c>
-      <c r="I19" s="8773" t="s">
+      <c r="I19" s="9196" t="s">
         <v>67</v>
       </c>
-      <c r="J19" s="8794" t="s">
+      <c r="J19" s="9217" t="s">
         <v>161</v>
       </c>
-      <c r="K19" s="8815" t="s">
+      <c r="K19" s="9238" t="s">
         <v>161</v>
       </c>
       <c r="U19" s="9"/>
@@ -37786,31 +39055,31 @@
     <row r="20">
       <c r="A20" s="24"/>
       <c r="B20"/>
-      <c r="C20" s="8651" t="s">
+      <c r="C20" s="9074" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="8672" t="s">
+      <c r="D20" s="9095" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="8691" t="s">
+      <c r="E20" s="9114" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="8711" t="s">
+      <c r="F20" s="9134" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="8732" t="s">
+      <c r="G20" s="9155" t="s">
         <v>162</v>
       </c>
-      <c r="H20" s="8753" t="s">
+      <c r="H20" s="9176" t="s">
         <v>163</v>
       </c>
-      <c r="I20" s="8774" t="s">
+      <c r="I20" s="9197" t="s">
         <v>67</v>
       </c>
-      <c r="J20" s="8795" t="s">
+      <c r="J20" s="9218" t="s">
         <v>164</v>
       </c>
-      <c r="K20" s="8816" t="s">
+      <c r="K20" s="9239" t="s">
         <v>164</v>
       </c>
       <c r="U20" s="9"/>
@@ -37824,31 +39093,31 @@
     <row r="21">
       <c r="A21" s="24"/>
       <c r="B21"/>
-      <c r="C21" s="8652" t="s">
+      <c r="C21" s="9075" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="8673" t="s">
+      <c r="D21" s="9096" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="8692" t="s">
+      <c r="E21" s="9115" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="8712" t="s">
+      <c r="F21" s="9135" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="8733" t="s">
+      <c r="G21" s="9156" t="s">
         <v>165</v>
       </c>
-      <c r="H21" s="8754" t="s">
+      <c r="H21" s="9177" t="s">
         <v>166</v>
       </c>
-      <c r="I21" s="8775" t="s">
+      <c r="I21" s="9198" t="s">
         <v>67</v>
       </c>
-      <c r="J21" s="8796" t="s">
+      <c r="J21" s="9219" t="s">
         <v>167</v>
       </c>
-      <c r="K21" s="8817" t="s">
+      <c r="K21" s="9240" t="s">
         <v>167</v>
       </c>
       <c r="U21" s="9"/>
@@ -37862,31 +39131,31 @@
     <row r="22">
       <c r="A22" s="24"/>
       <c r="B22"/>
-      <c r="C22" s="8653" t="s">
+      <c r="C22" s="9076" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="8674" t="s">
+      <c r="D22" s="9097" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="8693" t="s">
+      <c r="E22" s="9116" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="8713" t="s">
+      <c r="F22" s="9136" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="8734" t="s">
+      <c r="G22" s="9157" t="s">
         <v>168</v>
       </c>
-      <c r="H22" s="8755" t="s">
+      <c r="H22" s="9178" t="s">
         <v>169</v>
       </c>
-      <c r="I22" s="8776" t="s">
+      <c r="I22" s="9199" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="8797" t="s">
+      <c r="J22" s="9220" t="s">
         <v>170</v>
       </c>
-      <c r="K22" s="8818" t="s">
+      <c r="K22" s="9241" t="s">
         <v>170</v>
       </c>
       <c r="U22" s="9"/>
@@ -37900,29 +39169,29 @@
     <row r="23">
       <c r="A23" s="24"/>
       <c r="B23"/>
-      <c r="C23" s="8654" t="s">
+      <c r="C23" s="9077" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="8675" t="s">
+      <c r="D23" s="9098" t="s">
         <v>75</v>
       </c>
       <c r="E23" s="24"/>
-      <c r="F23" s="8714" t="s">
+      <c r="F23" s="9137" t="s">
         <v>128</v>
       </c>
-      <c r="G23" s="8735" t="s">
+      <c r="G23" s="9158" t="s">
         <v>171</v>
       </c>
-      <c r="H23" s="8756" t="s">
+      <c r="H23" s="9179" t="s">
         <v>172</v>
       </c>
-      <c r="I23" s="8777" t="s">
+      <c r="I23" s="9200" t="s">
         <v>67</v>
       </c>
-      <c r="J23" s="8798" t="s">
+      <c r="J23" s="9221" t="s">
         <v>173</v>
       </c>
-      <c r="K23" s="8819" t="s">
+      <c r="K23" s="9242" t="s">
         <v>173</v>
       </c>
       <c r="U23" s="9"/>
@@ -38908,28 +40177,28 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="8820" t="s">
+      <c r="C3" s="9243" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="8829" t="s">
+      <c r="D3" s="9252" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="8838" t="s">
+      <c r="E3" s="9261" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="8847" t="s">
+      <c r="F3" s="9270" t="s">
         <v>178</v>
       </c>
-      <c r="G3" s="8856" t="s">
+      <c r="G3" s="9279" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="8865" t="s">
+      <c r="H3" s="9288" t="s">
         <v>179</v>
       </c>
-      <c r="I3" s="8874" t="s">
+      <c r="I3" s="9297" t="s">
         <v>180</v>
       </c>
-      <c r="J3" s="8883" t="s">
+      <c r="J3" s="9306" t="s">
         <v>181</v>
       </c>
       <c r="K3"/>
@@ -38937,28 +40206,28 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="8821" t="s">
+      <c r="C4" s="9244" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="8830" t="s">
+      <c r="D4" s="9253" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="8839" t="s">
+      <c r="E4" s="9262" t="s">
         <v>182</v>
       </c>
-      <c r="F4" s="8848" t="s">
+      <c r="F4" s="9271" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="8857" t="s">
+      <c r="G4" s="9280" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="8866" t="s">
+      <c r="H4" s="9289" t="s">
         <v>184</v>
       </c>
-      <c r="I4" s="8875" t="s">
+      <c r="I4" s="9298" t="s">
         <v>185</v>
       </c>
-      <c r="J4" s="8884" t="s">
+      <c r="J4" s="9307" t="s">
         <v>186</v>
       </c>
       <c r="K4"/>
@@ -38966,28 +40235,28 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="8822" t="s">
+      <c r="C5" s="9245" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="8831" t="s">
+      <c r="D5" s="9254" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="8840" t="s">
+      <c r="E5" s="9263" t="s">
         <v>187</v>
       </c>
-      <c r="F5" s="8849" t="s">
+      <c r="F5" s="9272" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="8858" t="s">
+      <c r="G5" s="9281" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="8867" t="s">
+      <c r="H5" s="9290" t="s">
         <v>189</v>
       </c>
-      <c r="I5" s="8876" t="s">
+      <c r="I5" s="9299" t="s">
         <v>190</v>
       </c>
-      <c r="J5" s="8885" t="s">
+      <c r="J5" s="9308" t="s">
         <v>191</v>
       </c>
       <c r="K5"/>
@@ -38995,28 +40264,28 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="8823" t="s">
+      <c r="C6" s="9246" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="8832" t="s">
+      <c r="D6" s="9255" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="8841" t="s">
+      <c r="E6" s="9264" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="8850" t="s">
+      <c r="F6" s="9273" t="s">
         <v>193</v>
       </c>
-      <c r="G6" s="8859" t="s">
+      <c r="G6" s="9282" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="8868" t="s">
+      <c r="H6" s="9291" t="s">
         <v>194</v>
       </c>
-      <c r="I6" s="8877" t="s">
+      <c r="I6" s="9300" t="s">
         <v>195</v>
       </c>
-      <c r="J6" s="8886" t="s">
+      <c r="J6" s="9309" t="s">
         <v>196</v>
       </c>
       <c r="K6"/>
@@ -39024,28 +40293,28 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="8824" t="s">
+      <c r="C7" s="9247" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="8833" t="s">
+      <c r="D7" s="9256" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="8842" t="s">
+      <c r="E7" s="9265" t="s">
         <v>197</v>
       </c>
-      <c r="F7" s="8851" t="s">
+      <c r="F7" s="9274" t="s">
         <v>198</v>
       </c>
-      <c r="G7" s="8860" t="s">
+      <c r="G7" s="9283" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="8869" t="s">
+      <c r="H7" s="9292" t="s">
         <v>199</v>
       </c>
-      <c r="I7" s="8878" t="s">
+      <c r="I7" s="9301" t="s">
         <v>200</v>
       </c>
-      <c r="J7" s="8887" t="s">
+      <c r="J7" s="9310" t="s">
         <v>201</v>
       </c>
       <c r="K7"/>
@@ -39053,28 +40322,28 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="8825" t="s">
+      <c r="C8" s="9248" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="8834" t="s">
+      <c r="D8" s="9257" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="8843" t="s">
+      <c r="E8" s="9266" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="8852" t="s">
+      <c r="F8" s="9275" t="s">
         <v>203</v>
       </c>
-      <c r="G8" s="8861" t="s">
+      <c r="G8" s="9284" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="8870" t="s">
+      <c r="H8" s="9293" t="s">
         <v>204</v>
       </c>
-      <c r="I8" s="8879" t="s">
+      <c r="I8" s="9302" t="s">
         <v>205</v>
       </c>
-      <c r="J8" s="8888" t="s">
+      <c r="J8" s="9311" t="s">
         <v>206</v>
       </c>
       <c r="K8"/>
@@ -39082,28 +40351,28 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="8826" t="s">
+      <c r="C9" s="9249" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="8835" t="s">
+      <c r="D9" s="9258" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="8844" t="s">
+      <c r="E9" s="9267" t="s">
         <v>207</v>
       </c>
-      <c r="F9" s="8853" t="s">
+      <c r="F9" s="9276" t="s">
         <v>208</v>
       </c>
-      <c r="G9" s="8862" t="s">
+      <c r="G9" s="9285" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="8871" t="s">
+      <c r="H9" s="9294" t="s">
         <v>209</v>
       </c>
-      <c r="I9" s="8880" t="s">
+      <c r="I9" s="9303" t="s">
         <v>210</v>
       </c>
-      <c r="J9" s="8889" t="s">
+      <c r="J9" s="9312" t="s">
         <v>211</v>
       </c>
       <c r="K9"/>
@@ -39111,28 +40380,28 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="8827" t="s">
+      <c r="C10" s="9250" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="8836" t="s">
+      <c r="D10" s="9259" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="8845" t="s">
+      <c r="E10" s="9268" t="s">
         <v>212</v>
       </c>
-      <c r="F10" s="8854" t="s">
+      <c r="F10" s="9277" t="s">
         <v>213</v>
       </c>
-      <c r="G10" s="8863" t="s">
+      <c r="G10" s="9286" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="8872" t="s">
+      <c r="H10" s="9295" t="s">
         <v>214</v>
       </c>
-      <c r="I10" s="8881" t="s">
+      <c r="I10" s="9304" t="s">
         <v>215</v>
       </c>
-      <c r="J10" s="8890" t="s">
+      <c r="J10" s="9313" t="s">
         <v>216</v>
       </c>
       <c r="K10"/>
@@ -39140,28 +40409,28 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="8828" t="s">
+      <c r="C11" s="9251" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="8837" t="s">
+      <c r="D11" s="9260" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="8846" t="s">
+      <c r="E11" s="9269" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="8855" t="s">
+      <c r="F11" s="9278" t="s">
         <v>218</v>
       </c>
-      <c r="G11" s="8864" t="s">
+      <c r="G11" s="9287" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="8873" t="s">
+      <c r="H11" s="9296" t="s">
         <v>219</v>
       </c>
-      <c r="I11" s="8882" t="s">
+      <c r="I11" s="9305" t="s">
         <v>220</v>
       </c>
-      <c r="J11" s="8891" t="s">
+      <c r="J11" s="9314" t="s">
         <v>221</v>
       </c>
       <c r="K11"/>
@@ -39848,31 +41117,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="8892" t="s">
+      <c r="C3" s="9315" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="8898" t="s">
+      <c r="D3" s="9321" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="8904" t="s">
+      <c r="E3" s="9327" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="8910" t="s">
+      <c r="F3" s="9333" t="s">
         <v>224</v>
       </c>
-      <c r="G3" s="8916" t="s">
+      <c r="G3" s="9339" t="s">
         <v>225</v>
       </c>
-      <c r="H3" s="8922" t="s">
+      <c r="H3" s="9345" t="s">
         <v>226</v>
       </c>
-      <c r="I3" s="8928" t="s">
+      <c r="I3" s="9351" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="8934" t="s">
+      <c r="J3" s="9357" t="s">
         <v>227</v>
       </c>
-      <c r="K3" s="8940" t="s">
+      <c r="K3" s="9363" t="s">
         <v>228</v>
       </c>
       <c r="U3" s="9"/>
@@ -39888,31 +41157,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="8893" t="s">
+      <c r="C4" s="9316" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="8899" t="s">
+      <c r="D4" s="9322" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="8905" t="s">
+      <c r="E4" s="9328" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="8911" t="s">
+      <c r="F4" s="9334" t="s">
         <v>229</v>
       </c>
-      <c r="G4" s="8917" t="s">
+      <c r="G4" s="9340" t="s">
         <v>230</v>
       </c>
-      <c r="H4" s="8923" t="s">
+      <c r="H4" s="9346" t="s">
         <v>231</v>
       </c>
-      <c r="I4" s="8929" t="s">
+      <c r="I4" s="9352" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="8935" t="s">
+      <c r="J4" s="9358" t="s">
         <v>232</v>
       </c>
-      <c r="K4" s="8941" t="s">
+      <c r="K4" s="9364" t="s">
         <v>233</v>
       </c>
       <c r="U4" s="9"/>
@@ -39928,31 +41197,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="8894" t="s">
+      <c r="C5" s="9317" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="8900" t="s">
+      <c r="D5" s="9323" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="8906" t="s">
+      <c r="E5" s="9329" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="8912" t="s">
+      <c r="F5" s="9335" t="s">
         <v>224</v>
       </c>
-      <c r="G5" s="8918" t="s">
+      <c r="G5" s="9341" t="s">
         <v>234</v>
       </c>
-      <c r="H5" s="8924" t="s">
+      <c r="H5" s="9347" t="s">
         <v>235</v>
       </c>
-      <c r="I5" s="8930" t="s">
+      <c r="I5" s="9353" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="8936" t="s">
+      <c r="J5" s="9359" t="s">
         <v>236</v>
       </c>
-      <c r="K5" s="8942" t="s">
+      <c r="K5" s="9365" t="s">
         <v>228</v>
       </c>
       <c r="U5" s="9"/>
@@ -39968,31 +41237,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="8895" t="s">
+      <c r="C6" s="9318" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="8901" t="s">
+      <c r="D6" s="9324" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="8907" t="s">
+      <c r="E6" s="9330" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="8913" t="s">
+      <c r="F6" s="9336" t="s">
         <v>229</v>
       </c>
-      <c r="G6" s="8919" t="s">
+      <c r="G6" s="9342" t="s">
         <v>230</v>
       </c>
-      <c r="H6" s="8925" t="s">
+      <c r="H6" s="9348" t="s">
         <v>237</v>
       </c>
-      <c r="I6" s="8931" t="s">
+      <c r="I6" s="9354" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="8937" t="s">
+      <c r="J6" s="9360" t="s">
         <v>238</v>
       </c>
-      <c r="K6" s="8943" t="s">
+      <c r="K6" s="9366" t="s">
         <v>233</v>
       </c>
       <c r="U6" s="9"/>
@@ -40008,31 +41277,31 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="8896" t="s">
+      <c r="C7" s="9319" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="8902" t="s">
+      <c r="D7" s="9325" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="8908" t="s">
+      <c r="E7" s="9331" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="8914" t="s">
+      <c r="F7" s="9337" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="8920" t="s">
+      <c r="G7" s="9343" t="s">
         <v>239</v>
       </c>
-      <c r="H7" s="8926" t="s">
+      <c r="H7" s="9349" t="s">
         <v>240</v>
       </c>
-      <c r="I7" s="8932" t="s">
+      <c r="I7" s="9355" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="8938" t="s">
+      <c r="J7" s="9361" t="s">
         <v>241</v>
       </c>
-      <c r="K7" s="8944" t="s">
+      <c r="K7" s="9367" t="s">
         <v>242</v>
       </c>
       <c r="U7" s="9"/>
@@ -40048,31 +41317,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="8897" t="s">
+      <c r="C8" s="9320" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="8903" t="s">
+      <c r="D8" s="9326" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="8909" t="s">
+      <c r="E8" s="9332" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="8915" t="s">
+      <c r="F8" s="9338" t="s">
         <v>229</v>
       </c>
-      <c r="G8" s="8921" t="s">
+      <c r="G8" s="9344" t="s">
         <v>230</v>
       </c>
-      <c r="H8" s="8927" t="s">
+      <c r="H8" s="9350" t="s">
         <v>243</v>
       </c>
-      <c r="I8" s="8933" t="s">
+      <c r="I8" s="9356" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="8939" t="s">
+      <c r="J8" s="9362" t="s">
         <v>244</v>
       </c>
-      <c r="K8" s="8945" t="s">
+      <c r="K8" s="9368" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="9"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-06-29 15:32:45]  fix markdown relative link paths
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11611" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12034" uniqueCount="393">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1698,7 +1698,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10638">
+  <cellXfs count="11061">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1812,6 +1812,1275 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -41382,170 +42651,170 @@
       <c r="AA2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="10215" t="s">
+      <c r="A3" s="10638" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10223" t="s">
+      <c r="B3" s="10646" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="10231" t="s">
+      <c r="C3" s="10654" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="10239" t="s">
+      <c r="D3" s="10662" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="10247" t="s">
+      <c r="E3" s="10670" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="8986"/>
-      <c r="G3" t="s" s="10255">
+      <c r="G3" t="s" s="10678">
         <v>304</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10216" t="s">
+      <c r="A4" s="10639" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10224" t="s">
+      <c r="B4" s="10647" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="10232" t="s">
+      <c r="C4" s="10655" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="10240" t="s">
+      <c r="D4" s="10663" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="10248" t="s">
+      <c r="E4" s="10671" t="s">
         <v>43</v>
       </c>
       <c r="F4" s="8987"/>
-      <c r="G4" t="s" s="10256">
+      <c r="G4" t="s" s="10679">
         <v>305</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10217" t="s">
+      <c r="A5" s="10640" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10225" t="s">
+      <c r="B5" s="10648" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="10233" t="s">
+      <c r="C5" s="10656" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="10241" t="s">
+      <c r="D5" s="10664" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="10249" t="s">
+      <c r="E5" s="10672" t="s">
         <v>46</v>
       </c>
       <c r="F5" s="8988"/>
-      <c r="G5" t="s" s="10257">
+      <c r="G5" t="s" s="10680">
         <v>306</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10218" t="s">
+      <c r="A6" s="10641" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10226" t="s">
+      <c r="B6" s="10649" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="10234" t="s">
+      <c r="C6" s="10657" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="10242" t="s">
+      <c r="D6" s="10665" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="10250" t="s">
+      <c r="E6" s="10673" t="s">
         <v>48</v>
       </c>
       <c r="F6" s="8989"/>
-      <c r="G6" t="s" s="10258">
+      <c r="G6" t="s" s="10681">
         <v>307</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10219" t="s">
+      <c r="A7" s="10642" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="10227" t="s">
+      <c r="B7" s="10650" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="10235" t="s">
+      <c r="C7" s="10658" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="10243" t="s">
+      <c r="D7" s="10666" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="10251" t="s">
+      <c r="E7" s="10674" t="s">
         <v>50</v>
       </c>
       <c r="F7" s="8990"/>
-      <c r="G7" t="s" s="10259">
+      <c r="G7" t="s" s="10682">
         <v>308</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10220" t="s">
+      <c r="A8" s="10643" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="10228" t="s">
+      <c r="B8" s="10651" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="10236" t="s">
+      <c r="C8" s="10659" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="10244" t="s">
+      <c r="D8" s="10667" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="10252" t="s">
+      <c r="E8" s="10675" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="8991"/>
-      <c r="G8" t="s" s="10260">
+      <c r="G8" t="s" s="10683">
         <v>309</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="10221" t="s">
+      <c r="A9" s="10644" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="10229" t="s">
+      <c r="B9" s="10652" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="10237" t="s">
+      <c r="C9" s="10660" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="10245" t="s">
+      <c r="D9" s="10668" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="10253" t="s">
+      <c r="E9" s="10676" t="s">
         <v>54</v>
       </c>
       <c r="F9" s="8992"/>
-      <c r="G9" t="s" s="10261">
+      <c r="G9" t="s" s="10684">
         <v>310</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10222" t="s">
+      <c r="A10" s="10645" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="10230" t="s">
+      <c r="B10" s="10653" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="10238" t="s">
+      <c r="C10" s="10661" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="10246" t="s">
+      <c r="D10" s="10669" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="10254" t="s">
+      <c r="E10" s="10677" t="s">
         <v>56</v>
       </c>
       <c r="F10" s="8993"/>
-      <c r="G10" t="s" s="10262">
+      <c r="G10" t="s" s="10685">
         <v>311</v>
       </c>
     </row>
@@ -41673,243 +42942,243 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="10263" t="s">
+      <c r="C3" s="10686" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="10272" t="s">
+      <c r="D3" s="10695" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="10281" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="10290" t="s">
+      <c r="E3" s="10704" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="10713" t="s">
         <v>66</v>
       </c>
       <c r="G3" s="9030"/>
-      <c r="H3" s="10299" t="s">
+      <c r="H3" s="10722" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="10308" t="s">
+      <c r="I3" s="10731" t="s">
         <v>69</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="10317">
+      <c r="K3" t="s" s="10740">
         <v>312</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="10264" t="s">
+      <c r="C4" s="10687" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="10273" t="s">
+      <c r="D4" s="10696" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="10282" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="10291" t="s">
+      <c r="E4" s="10705" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="10714" t="s">
         <v>72</v>
       </c>
       <c r="G4" s="9031"/>
-      <c r="H4" s="10300" t="s">
+      <c r="H4" s="10723" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="10309" t="s">
+      <c r="I4" s="10732" t="s">
         <v>74</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="10318">
+      <c r="K4" t="s" s="10741">
         <v>313</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="10265" t="s">
+      <c r="C5" s="10688" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="10274" t="s">
+      <c r="D5" s="10697" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="10283" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="10292" t="s">
+      <c r="E5" s="10706" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="10715" t="s">
         <v>77</v>
       </c>
       <c r="G5" s="9032"/>
-      <c r="H5" s="10301" t="s">
+      <c r="H5" s="10724" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="10310" t="s">
+      <c r="I5" s="10733" t="s">
         <v>79</v>
       </c>
       <c r="J5"/>
-      <c r="K5" t="s" s="10319">
+      <c r="K5" t="s" s="10742">
         <v>314</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="10266" t="s">
+      <c r="C6" s="10689" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="10275" t="s">
+      <c r="D6" s="10698" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="10284" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="10293" t="s">
+      <c r="E6" s="10707" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="10716" t="s">
         <v>81</v>
       </c>
       <c r="G6" s="9033"/>
-      <c r="H6" s="10302" t="s">
+      <c r="H6" s="10725" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="10311" t="s">
+      <c r="I6" s="10734" t="s">
         <v>83</v>
       </c>
       <c r="J6"/>
-      <c r="K6" t="s" s="10320">
+      <c r="K6" t="s" s="10743">
         <v>315</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="10267" t="s">
+      <c r="C7" s="10690" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="10276" t="s">
+      <c r="D7" s="10699" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="10285" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="10294" t="s">
+      <c r="E7" s="10708" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="10717" t="s">
         <v>85</v>
       </c>
       <c r="G7" s="9034"/>
-      <c r="H7" s="10303" t="s">
+      <c r="H7" s="10726" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="10312" t="s">
+      <c r="I7" s="10735" t="s">
         <v>87</v>
       </c>
       <c r="J7"/>
-      <c r="K7" t="s" s="10321">
+      <c r="K7" t="s" s="10744">
         <v>316</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="10268" t="s">
+      <c r="C8" s="10691" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="10277" t="s">
+      <c r="D8" s="10700" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="10286" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="10295" t="s">
+      <c r="E8" s="10709" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="10718" t="s">
         <v>89</v>
       </c>
       <c r="G8" s="9035"/>
-      <c r="H8" s="10304" t="s">
+      <c r="H8" s="10727" t="s">
         <v>90</v>
       </c>
-      <c r="I8" s="10313" t="s">
+      <c r="I8" s="10736" t="s">
         <v>91</v>
       </c>
       <c r="J8"/>
-      <c r="K8" t="s" s="10322">
+      <c r="K8" t="s" s="10745">
         <v>317</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="10269" t="s">
+      <c r="C9" s="10692" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="10278" t="s">
+      <c r="D9" s="10701" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="10287" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="10296" t="s">
+      <c r="E9" s="10710" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="10719" t="s">
         <v>93</v>
       </c>
       <c r="G9" s="9036"/>
-      <c r="H9" s="10305" t="s">
+      <c r="H9" s="10728" t="s">
         <v>94</v>
       </c>
-      <c r="I9" s="10314" t="s">
+      <c r="I9" s="10737" t="s">
         <v>95</v>
       </c>
       <c r="J9"/>
-      <c r="K9" t="s" s="10323">
+      <c r="K9" t="s" s="10746">
         <v>318</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="10270" t="s">
+      <c r="C10" s="10693" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="10279" t="s">
+      <c r="D10" s="10702" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="10288" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="10297" t="s">
+      <c r="E10" s="10711" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="10720" t="s">
         <v>97</v>
       </c>
       <c r="G10" s="9037"/>
-      <c r="H10" s="10306" t="s">
+      <c r="H10" s="10729" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="10315" t="s">
+      <c r="I10" s="10738" t="s">
         <v>99</v>
       </c>
       <c r="J10"/>
-      <c r="K10" t="s" s="10324">
+      <c r="K10" t="s" s="10747">
         <v>319</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="10271" t="s">
+      <c r="C11" s="10694" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="10280" t="s">
+      <c r="D11" s="10703" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="10289" t="s">
-        <v>96</v>
-      </c>
-      <c r="F11" s="10298" t="s">
+      <c r="E11" s="10712" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="10721" t="s">
         <v>101</v>
       </c>
       <c r="G11" s="9038"/>
-      <c r="H11" s="10307" t="s">
+      <c r="H11" s="10730" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="10316" t="s">
+      <c r="I11" s="10739" t="s">
         <v>103</v>
       </c>
       <c r="J11"/>
-      <c r="K11" t="s" s="10325">
+      <c r="K11" t="s" s="10748">
         <v>320</v>
       </c>
     </row>
@@ -42504,32 +43773,32 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="10326" t="s">
+      <c r="C3" s="10749" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="10347" t="s">
+      <c r="D3" s="10770" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="10368" t="s">
+      <c r="E3" s="10791" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="10386" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="10407" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" s="10428" t="s">
+      <c r="F3" s="10809" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10830" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="10851" t="s">
         <v>110</v>
       </c>
       <c r="I3" s="9180"/>
-      <c r="J3" s="10449" t="s">
+      <c r="J3" s="10872" t="s">
         <v>321</v>
       </c>
-      <c r="K3" s="10470" t="s">
+      <c r="K3" s="10893" t="s">
         <v>111</v>
       </c>
-      <c r="L3" t="s" s="10491">
+      <c r="L3" t="s" s="10914">
         <v>345</v>
       </c>
       <c r="U3" s="9"/>
@@ -42543,32 +43812,32 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="10327" t="s">
+      <c r="C4" s="10750" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="10348" t="s">
+      <c r="D4" s="10771" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="10369" t="s">
+      <c r="E4" s="10792" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="10387" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="10408" t="s">
-        <v>113</v>
-      </c>
-      <c r="H4" s="10429" t="s">
+      <c r="F4" s="10810" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="10831" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="10852" t="s">
         <v>114</v>
       </c>
       <c r="I4" s="9181"/>
-      <c r="J4" s="10450" t="s">
+      <c r="J4" s="10873" t="s">
         <v>322</v>
       </c>
-      <c r="K4" s="10471" t="s">
+      <c r="K4" s="10894" t="s">
         <v>115</v>
       </c>
-      <c r="L4" t="s" s="10492">
+      <c r="L4" t="s" s="10915">
         <v>346</v>
       </c>
       <c r="U4" s="9"/>
@@ -42582,32 +43851,32 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="10328" t="s">
+      <c r="C5" s="10751" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="10349" t="s">
+      <c r="D5" s="10772" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="10370" t="s">
+      <c r="E5" s="10793" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="10388" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="10409" t="s">
-        <v>125</v>
-      </c>
-      <c r="H5" s="10430" t="s">
+      <c r="F5" s="10811" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="10832" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="10853" t="s">
         <v>117</v>
       </c>
       <c r="I5" s="9182"/>
-      <c r="J5" s="10451" t="s">
+      <c r="J5" s="10874" t="s">
         <v>323</v>
       </c>
-      <c r="K5" s="10472" t="s">
+      <c r="K5" s="10895" t="s">
         <v>118</v>
       </c>
-      <c r="L5" t="s" s="10493">
+      <c r="L5" t="s" s="10916">
         <v>347</v>
       </c>
       <c r="U5" s="9"/>
@@ -42621,32 +43890,32 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="10329" t="s">
+      <c r="C6" s="10752" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="10350" t="s">
+      <c r="D6" s="10773" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="10371" t="s">
+      <c r="E6" s="10794" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="10389" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="10410" t="s">
-        <v>122</v>
-      </c>
-      <c r="H6" s="10431" t="s">
+      <c r="F6" s="10812" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="10833" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="10854" t="s">
         <v>120</v>
       </c>
       <c r="I6" s="9183"/>
-      <c r="J6" s="10452" t="s">
+      <c r="J6" s="10875" t="s">
         <v>324</v>
       </c>
-      <c r="K6" s="10473" t="s">
+      <c r="K6" s="10896" t="s">
         <v>121</v>
       </c>
-      <c r="L6" t="s" s="10494">
+      <c r="L6" t="s" s="10917">
         <v>348</v>
       </c>
       <c r="U6" s="9"/>
@@ -42660,32 +43929,32 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="10330" t="s">
+      <c r="C7" s="10753" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="10351" t="s">
+      <c r="D7" s="10774" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="10372" t="s">
+      <c r="E7" s="10795" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="10390" t="s">
+      <c r="F7" s="10813" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="10411" t="s">
-        <v>119</v>
-      </c>
-      <c r="H7" s="10432" t="s">
+      <c r="G7" s="10834" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="10855" t="s">
         <v>123</v>
       </c>
       <c r="I7" s="9184"/>
-      <c r="J7" s="10453" t="s">
+      <c r="J7" s="10876" t="s">
         <v>325</v>
       </c>
-      <c r="K7" s="10474" t="s">
+      <c r="K7" s="10897" t="s">
         <v>124</v>
       </c>
-      <c r="L7" t="s" s="10495">
+      <c r="L7" t="s" s="10918">
         <v>349</v>
       </c>
       <c r="U7" s="9"/>
@@ -42699,32 +43968,32 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="10331" t="s">
+      <c r="C8" s="10754" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="10352" t="s">
+      <c r="D8" s="10775" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="10373" t="s">
+      <c r="E8" s="10796" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="10391" t="s">
+      <c r="F8" s="10814" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="10412" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" s="10433" t="s">
+      <c r="G8" s="10835" t="s">
+        <v>144</v>
+      </c>
+      <c r="H8" s="10856" t="s">
         <v>126</v>
       </c>
       <c r="I8" s="9185"/>
-      <c r="J8" s="10454" t="s">
+      <c r="J8" s="10877" t="s">
         <v>326</v>
       </c>
-      <c r="K8" s="10475" t="s">
+      <c r="K8" s="10898" t="s">
         <v>127</v>
       </c>
-      <c r="L8" t="s" s="10496">
+      <c r="L8" t="s" s="10919">
         <v>350</v>
       </c>
       <c r="U8" s="9"/>
@@ -42738,30 +44007,30 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="10332" t="s">
+      <c r="C9" s="10755" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="10353" t="s">
+      <c r="D9" s="10776" t="s">
         <v>75</v>
       </c>
       <c r="E9" s="24"/>
-      <c r="F9" s="10392" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="10413" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" s="10434" t="s">
+      <c r="F9" s="10815" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="10836" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" s="10857" t="s">
         <v>130</v>
       </c>
       <c r="I9" s="9186"/>
-      <c r="J9" s="10455" t="s">
+      <c r="J9" s="10878" t="s">
         <v>327</v>
       </c>
-      <c r="K9" s="10476" t="s">
+      <c r="K9" s="10899" t="s">
         <v>342</v>
       </c>
-      <c r="L9" t="s" s="10497">
+      <c r="L9" t="s" s="10920">
         <v>351</v>
       </c>
       <c r="U9" s="9"/>
@@ -42775,32 +44044,32 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="10333" t="s">
+      <c r="C10" s="10756" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="10354" t="s">
+      <c r="D10" s="10777" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="10374" t="s">
+      <c r="E10" s="10797" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="10393" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="10414" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="10435" t="s">
+      <c r="F10" s="10816" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="10837" t="s">
+        <v>162</v>
+      </c>
+      <c r="H10" s="10858" t="s">
         <v>133</v>
       </c>
       <c r="I10" s="9187"/>
-      <c r="J10" s="10456" t="s">
+      <c r="J10" s="10879" t="s">
         <v>328</v>
       </c>
-      <c r="K10" s="10477" t="s">
+      <c r="K10" s="10900" t="s">
         <v>134</v>
       </c>
-      <c r="L10" t="s" s="10498">
+      <c r="L10" t="s" s="10921">
         <v>352</v>
       </c>
       <c r="U10" s="9"/>
@@ -42814,32 +44083,32 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="10334" t="s">
+      <c r="C11" s="10757" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="10355" t="s">
+      <c r="D11" s="10778" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="10375" t="s">
+      <c r="E11" s="10798" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="10394" t="s">
-        <v>128</v>
-      </c>
-      <c r="G11" s="10415" t="s">
-        <v>150</v>
-      </c>
-      <c r="H11" s="10436" t="s">
+      <c r="F11" s="10817" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="10838" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="10859" t="s">
         <v>136</v>
       </c>
       <c r="I11" s="9188"/>
-      <c r="J11" s="10457" t="s">
+      <c r="J11" s="10880" t="s">
         <v>329</v>
       </c>
-      <c r="K11" s="10478" t="s">
+      <c r="K11" s="10901" t="s">
         <v>137</v>
       </c>
-      <c r="L11" t="s" s="10499">
+      <c r="L11" t="s" s="10922">
         <v>353</v>
       </c>
       <c r="U11" s="9"/>
@@ -42853,32 +44122,32 @@
     <row r="12">
       <c r="A12" s="24"/>
       <c r="B12"/>
-      <c r="C12" s="10335" t="s">
+      <c r="C12" s="10758" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="10356" t="s">
+      <c r="D12" s="10779" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="10376" t="s">
+      <c r="E12" s="10799" t="s">
         <v>108</v>
       </c>
-      <c r="F12" s="10395" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="10416" t="s">
-        <v>144</v>
-      </c>
-      <c r="H12" s="10437" t="s">
+      <c r="F12" s="10818" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="10839" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" s="10860" t="s">
         <v>139</v>
       </c>
       <c r="I12" s="9189"/>
-      <c r="J12" s="10458" t="s">
+      <c r="J12" s="10881" t="s">
         <v>330</v>
       </c>
-      <c r="K12" s="10479" t="s">
+      <c r="K12" s="10902" t="s">
         <v>140</v>
       </c>
-      <c r="L12" t="s" s="10500">
+      <c r="L12" t="s" s="10923">
         <v>354</v>
       </c>
       <c r="U12" s="9"/>
@@ -42892,32 +44161,32 @@
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13"/>
-      <c r="C13" s="10336" t="s">
+      <c r="C13" s="10759" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="10357" t="s">
+      <c r="D13" s="10780" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="10377" t="s">
+      <c r="E13" s="10800" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="10396" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="10417" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" s="10438" t="s">
+      <c r="F13" s="10819" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="10840" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" s="10861" t="s">
         <v>142</v>
       </c>
       <c r="I13" s="9190"/>
-      <c r="J13" s="10459" t="s">
+      <c r="J13" s="10882" t="s">
         <v>331</v>
       </c>
-      <c r="K13" s="10480" t="s">
+      <c r="K13" s="10903" t="s">
         <v>143</v>
       </c>
-      <c r="L13" t="s" s="10501">
+      <c r="L13" t="s" s="10924">
         <v>355</v>
       </c>
       <c r="U13" s="9"/>
@@ -42931,32 +44200,32 @@
     <row r="14">
       <c r="A14" s="24"/>
       <c r="B14"/>
-      <c r="C14" s="10337" t="s">
+      <c r="C14" s="10760" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="10358" t="s">
+      <c r="D14" s="10781" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="10378" t="s">
+      <c r="E14" s="10801" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="10397" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="10418" t="s">
-        <v>138</v>
-      </c>
-      <c r="H14" s="10439" t="s">
+      <c r="F14" s="10820" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="10841" t="s">
+        <v>168</v>
+      </c>
+      <c r="H14" s="10862" t="s">
         <v>145</v>
       </c>
       <c r="I14" s="9191"/>
-      <c r="J14" s="10460" t="s">
+      <c r="J14" s="10883" t="s">
         <v>332</v>
       </c>
-      <c r="K14" s="10481" t="s">
+      <c r="K14" s="10904" t="s">
         <v>146</v>
       </c>
-      <c r="L14" t="s" s="10502">
+      <c r="L14" t="s" s="10925">
         <v>356</v>
       </c>
       <c r="U14" s="9"/>
@@ -42970,32 +44239,32 @@
     <row r="15">
       <c r="A15" s="24"/>
       <c r="B15"/>
-      <c r="C15" s="10338" t="s">
+      <c r="C15" s="10761" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="10359" t="s">
+      <c r="D15" s="10782" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="10379" t="s">
+      <c r="E15" s="10802" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="10398" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="10419" t="s">
-        <v>141</v>
-      </c>
-      <c r="H15" s="10440" t="s">
+      <c r="F15" s="10821" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="10842" t="s">
+        <v>165</v>
+      </c>
+      <c r="H15" s="10863" t="s">
         <v>148</v>
       </c>
       <c r="I15" s="9192"/>
-      <c r="J15" s="10461" t="s">
+      <c r="J15" s="10884" t="s">
         <v>333</v>
       </c>
-      <c r="K15" s="10482" t="s">
+      <c r="K15" s="10905" t="s">
         <v>149</v>
       </c>
-      <c r="L15" t="s" s="10503">
+      <c r="L15" t="s" s="10926">
         <v>357</v>
       </c>
       <c r="U15" s="9"/>
@@ -43009,30 +44278,30 @@
     <row r="16">
       <c r="A16" s="24"/>
       <c r="B16"/>
-      <c r="C16" s="10339" t="s">
+      <c r="C16" s="10762" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="10360" t="s">
+      <c r="D16" s="10783" t="s">
         <v>75</v>
       </c>
       <c r="E16" s="24"/>
-      <c r="F16" s="10399" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="10420" t="s">
-        <v>135</v>
-      </c>
-      <c r="H16" s="10441" t="s">
+      <c r="F16" s="10822" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" s="10843" t="s">
+        <v>171</v>
+      </c>
+      <c r="H16" s="10864" t="s">
         <v>151</v>
       </c>
       <c r="I16" s="9193"/>
-      <c r="J16" s="10462" t="s">
+      <c r="J16" s="10885" t="s">
         <v>334</v>
       </c>
-      <c r="K16" s="10483" t="s">
+      <c r="K16" s="10906" t="s">
         <v>343</v>
       </c>
-      <c r="L16" t="s" s="10504">
+      <c r="L16" t="s" s="10927">
         <v>358</v>
       </c>
       <c r="U16" s="9"/>
@@ -43046,32 +44315,32 @@
     <row r="17">
       <c r="A17" s="24"/>
       <c r="B17"/>
-      <c r="C17" s="10340" t="s">
+      <c r="C17" s="10763" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="10361" t="s">
+      <c r="D17" s="10784" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="10380" t="s">
+      <c r="E17" s="10803" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="10400" t="s">
-        <v>128</v>
-      </c>
-      <c r="G17" s="10421" t="s">
-        <v>171</v>
-      </c>
-      <c r="H17" s="10442" t="s">
+      <c r="F17" s="10823" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="10844" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="10865" t="s">
         <v>154</v>
       </c>
       <c r="I17" s="9194"/>
-      <c r="J17" s="10463" t="s">
+      <c r="J17" s="10886" t="s">
         <v>335</v>
       </c>
-      <c r="K17" s="10484" t="s">
+      <c r="K17" s="10907" t="s">
         <v>155</v>
       </c>
-      <c r="L17" t="s" s="10505">
+      <c r="L17" t="s" s="10928">
         <v>359</v>
       </c>
       <c r="U17" s="9"/>
@@ -43085,32 +44354,32 @@
     <row r="18">
       <c r="A18" s="24"/>
       <c r="B18"/>
-      <c r="C18" s="10341" t="s">
+      <c r="C18" s="10764" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="10362" t="s">
+      <c r="D18" s="10785" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="10381" t="s">
+      <c r="E18" s="10804" t="s">
         <v>112</v>
       </c>
-      <c r="F18" s="10401" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="10422" t="s">
-        <v>168</v>
-      </c>
-      <c r="H18" s="10443" t="s">
+      <c r="F18" s="10824" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="10845" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="10866" t="s">
         <v>157</v>
       </c>
       <c r="I18" s="9195"/>
-      <c r="J18" s="10464" t="s">
+      <c r="J18" s="10887" t="s">
         <v>336</v>
       </c>
-      <c r="K18" s="10485" t="s">
+      <c r="K18" s="10908" t="s">
         <v>158</v>
       </c>
-      <c r="L18" t="s" s="10506">
+      <c r="L18" t="s" s="10929">
         <v>360</v>
       </c>
       <c r="U18" s="9"/>
@@ -43124,32 +44393,32 @@
     <row r="19">
       <c r="A19" s="24"/>
       <c r="B19"/>
-      <c r="C19" s="10342" t="s">
+      <c r="C19" s="10765" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="10363" t="s">
+      <c r="D19" s="10786" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="10382" t="s">
+      <c r="E19" s="10805" t="s">
         <v>108</v>
       </c>
-      <c r="F19" s="10402" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="10423" t="s">
-        <v>165</v>
-      </c>
-      <c r="H19" s="10444" t="s">
+      <c r="F19" s="10825" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="10846" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" s="10867" t="s">
         <v>160</v>
       </c>
       <c r="I19" s="9196"/>
-      <c r="J19" s="10465" t="s">
+      <c r="J19" s="10888" t="s">
         <v>337</v>
       </c>
-      <c r="K19" s="10486" t="s">
+      <c r="K19" s="10909" t="s">
         <v>161</v>
       </c>
-      <c r="L19" t="s" s="10507">
+      <c r="L19" t="s" s="10930">
         <v>361</v>
       </c>
       <c r="U19" s="9"/>
@@ -43163,32 +44432,32 @@
     <row r="20">
       <c r="A20" s="24"/>
       <c r="B20"/>
-      <c r="C20" s="10343" t="s">
+      <c r="C20" s="10766" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="10364" t="s">
+      <c r="D20" s="10787" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="10383" t="s">
+      <c r="E20" s="10806" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="10403" t="s">
+      <c r="F20" s="10826" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="10424" t="s">
-        <v>162</v>
-      </c>
-      <c r="H20" s="10445" t="s">
+      <c r="G20" s="10847" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="10868" t="s">
         <v>163</v>
       </c>
       <c r="I20" s="9197"/>
-      <c r="J20" s="10466" t="s">
+      <c r="J20" s="10889" t="s">
         <v>338</v>
       </c>
-      <c r="K20" s="10487" t="s">
+      <c r="K20" s="10910" t="s">
         <v>164</v>
       </c>
-      <c r="L20" t="s" s="10508">
+      <c r="L20" t="s" s="10931">
         <v>362</v>
       </c>
       <c r="U20" s="9"/>
@@ -43202,32 +44471,32 @@
     <row r="21">
       <c r="A21" s="24"/>
       <c r="B21"/>
-      <c r="C21" s="10344" t="s">
+      <c r="C21" s="10767" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="10365" t="s">
+      <c r="D21" s="10788" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="10384" t="s">
+      <c r="E21" s="10807" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="10404" t="s">
+      <c r="F21" s="10827" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="10425" t="s">
-        <v>159</v>
-      </c>
-      <c r="H21" s="10446" t="s">
+      <c r="G21" s="10848" t="s">
+        <v>122</v>
+      </c>
+      <c r="H21" s="10869" t="s">
         <v>166</v>
       </c>
       <c r="I21" s="9198"/>
-      <c r="J21" s="10467" t="s">
+      <c r="J21" s="10890" t="s">
         <v>339</v>
       </c>
-      <c r="K21" s="10488" t="s">
+      <c r="K21" s="10911" t="s">
         <v>167</v>
       </c>
-      <c r="L21" t="s" s="10509">
+      <c r="L21" t="s" s="10932">
         <v>363</v>
       </c>
       <c r="U21" s="9"/>
@@ -43241,32 +44510,32 @@
     <row r="22">
       <c r="A22" s="24"/>
       <c r="B22"/>
-      <c r="C22" s="10345" t="s">
+      <c r="C22" s="10768" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="10366" t="s">
+      <c r="D22" s="10789" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="10385" t="s">
+      <c r="E22" s="10808" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="10405" t="s">
+      <c r="F22" s="10828" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="10426" t="s">
-        <v>156</v>
-      </c>
-      <c r="H22" s="10447" t="s">
+      <c r="G22" s="10849" t="s">
+        <v>125</v>
+      </c>
+      <c r="H22" s="10870" t="s">
         <v>169</v>
       </c>
       <c r="I22" s="9199"/>
-      <c r="J22" s="10468" t="s">
+      <c r="J22" s="10891" t="s">
         <v>340</v>
       </c>
-      <c r="K22" s="10489" t="s">
+      <c r="K22" s="10912" t="s">
         <v>170</v>
       </c>
-      <c r="L22" t="s" s="10510">
+      <c r="L22" t="s" s="10933">
         <v>364</v>
       </c>
       <c r="U22" s="9"/>
@@ -43280,30 +44549,30 @@
     <row r="23">
       <c r="A23" s="24"/>
       <c r="B23"/>
-      <c r="C23" s="10346" t="s">
+      <c r="C23" s="10769" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="10367" t="s">
+      <c r="D23" s="10790" t="s">
         <v>75</v>
       </c>
       <c r="E23" s="24"/>
-      <c r="F23" s="10406" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="10427" t="s">
-        <v>153</v>
-      </c>
-      <c r="H23" s="10448" t="s">
+      <c r="F23" s="10829" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="10850" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="10871" t="s">
         <v>172</v>
       </c>
       <c r="I23" s="9200"/>
-      <c r="J23" s="10469" t="s">
+      <c r="J23" s="10892" t="s">
         <v>341</v>
       </c>
-      <c r="K23" s="10490" t="s">
+      <c r="K23" s="10913" t="s">
         <v>344</v>
       </c>
-      <c r="L23" t="s" s="10511">
+      <c r="L23" t="s" s="10934">
         <v>365</v>
       </c>
       <c r="U23" s="9"/>
@@ -44289,270 +45558,270 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="10512" t="s">
+      <c r="C3" s="10935" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="10521" t="s">
+      <c r="D3" s="10944" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="10530" t="s">
+      <c r="E3" s="10953" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="10539" t="s">
+      <c r="F3" s="10962" t="s">
         <v>178</v>
       </c>
       <c r="G3" s="9279"/>
-      <c r="H3" s="10548" t="s">
+      <c r="H3" s="10971" t="s">
         <v>179</v>
       </c>
-      <c r="I3" s="10557" t="s">
+      <c r="I3" s="10980" t="s">
         <v>180</v>
       </c>
-      <c r="J3" s="10566" t="s">
+      <c r="J3" s="10989" t="s">
         <v>181</v>
       </c>
       <c r="K3"/>
-      <c r="L3" t="s" s="10575">
+      <c r="L3" t="s" s="10998">
         <v>366</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="10513" t="s">
+      <c r="C4" s="10936" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="10522" t="s">
+      <c r="D4" s="10945" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="10531" t="s">
-        <v>187</v>
-      </c>
-      <c r="F4" s="10540" t="s">
+      <c r="E4" s="10954" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="10963" t="s">
         <v>183</v>
       </c>
       <c r="G4" s="9280"/>
-      <c r="H4" s="10549" t="s">
+      <c r="H4" s="10972" t="s">
         <v>184</v>
       </c>
-      <c r="I4" s="10558" t="s">
-        <v>190</v>
-      </c>
-      <c r="J4" s="10567" t="s">
-        <v>191</v>
+      <c r="I4" s="10981" t="s">
+        <v>185</v>
+      </c>
+      <c r="J4" s="10990" t="s">
+        <v>186</v>
       </c>
       <c r="K4"/>
-      <c r="L4" t="s" s="10576">
+      <c r="L4" t="s" s="10999">
         <v>367</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="10514" t="s">
+      <c r="C5" s="10937" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="10523" t="s">
+      <c r="D5" s="10946" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="10532" t="s">
-        <v>182</v>
-      </c>
-      <c r="F5" s="10541" t="s">
+      <c r="E5" s="10955" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="10964" t="s">
         <v>188</v>
       </c>
       <c r="G5" s="9281"/>
-      <c r="H5" s="10550" t="s">
+      <c r="H5" s="10973" t="s">
         <v>189</v>
       </c>
-      <c r="I5" s="10559" t="s">
-        <v>185</v>
-      </c>
-      <c r="J5" s="10568" t="s">
-        <v>186</v>
+      <c r="I5" s="10982" t="s">
+        <v>190</v>
+      </c>
+      <c r="J5" s="10991" t="s">
+        <v>191</v>
       </c>
       <c r="K5"/>
-      <c r="L5" t="s" s="10577">
+      <c r="L5" t="s" s="11000">
         <v>368</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="10515" t="s">
+      <c r="C6" s="10938" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="10524" t="s">
+      <c r="D6" s="10947" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="10533" t="s">
-        <v>207</v>
-      </c>
-      <c r="F6" s="10542" t="s">
+      <c r="E6" s="10956" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" s="10965" t="s">
         <v>193</v>
       </c>
       <c r="G6" s="9282"/>
-      <c r="H6" s="10551" t="s">
+      <c r="H6" s="10974" t="s">
         <v>194</v>
       </c>
-      <c r="I6" s="10560" t="s">
-        <v>210</v>
-      </c>
-      <c r="J6" s="10569" t="s">
-        <v>211</v>
+      <c r="I6" s="10983" t="s">
+        <v>195</v>
+      </c>
+      <c r="J6" s="10992" t="s">
+        <v>196</v>
       </c>
       <c r="K6"/>
-      <c r="L6" t="s" s="10578">
+      <c r="L6" t="s" s="11001">
         <v>369</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="10516" t="s">
+      <c r="C7" s="10939" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="10525" t="s">
+      <c r="D7" s="10948" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="10534" t="s">
-        <v>217</v>
-      </c>
-      <c r="F7" s="10543" t="s">
+      <c r="E7" s="10957" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" s="10966" t="s">
         <v>198</v>
       </c>
       <c r="G7" s="9283"/>
-      <c r="H7" s="10552" t="s">
+      <c r="H7" s="10975" t="s">
         <v>199</v>
       </c>
-      <c r="I7" s="10561" t="s">
-        <v>220</v>
-      </c>
-      <c r="J7" s="10570" t="s">
-        <v>221</v>
+      <c r="I7" s="10984" t="s">
+        <v>200</v>
+      </c>
+      <c r="J7" s="10993" t="s">
+        <v>201</v>
       </c>
       <c r="K7"/>
-      <c r="L7" t="s" s="10579">
+      <c r="L7" t="s" s="11002">
         <v>370</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="10517" t="s">
+      <c r="C8" s="10940" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="10526" t="s">
+      <c r="D8" s="10949" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="10535" t="s">
-        <v>212</v>
-      </c>
-      <c r="F8" s="10544" t="s">
+      <c r="E8" s="10958" t="s">
+        <v>202</v>
+      </c>
+      <c r="F8" s="10967" t="s">
         <v>203</v>
       </c>
       <c r="G8" s="9284"/>
-      <c r="H8" s="10553" t="s">
+      <c r="H8" s="10976" t="s">
         <v>204</v>
       </c>
-      <c r="I8" s="10562" t="s">
-        <v>215</v>
-      </c>
-      <c r="J8" s="10571" t="s">
-        <v>216</v>
+      <c r="I8" s="10985" t="s">
+        <v>205</v>
+      </c>
+      <c r="J8" s="10994" t="s">
+        <v>206</v>
       </c>
       <c r="K8"/>
-      <c r="L8" t="s" s="10580">
+      <c r="L8" t="s" s="11003">
         <v>371</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="10518" t="s">
+      <c r="C9" s="10941" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="10527" t="s">
+      <c r="D9" s="10950" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="10536" t="s">
-        <v>202</v>
-      </c>
-      <c r="F9" s="10545" t="s">
+      <c r="E9" s="10959" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" s="10968" t="s">
         <v>208</v>
       </c>
       <c r="G9" s="9285"/>
-      <c r="H9" s="10554" t="s">
+      <c r="H9" s="10977" t="s">
         <v>209</v>
       </c>
-      <c r="I9" s="10563" t="s">
-        <v>205</v>
-      </c>
-      <c r="J9" s="10572" t="s">
-        <v>206</v>
+      <c r="I9" s="10986" t="s">
+        <v>210</v>
+      </c>
+      <c r="J9" s="10995" t="s">
+        <v>211</v>
       </c>
       <c r="K9"/>
-      <c r="L9" t="s" s="10581">
+      <c r="L9" t="s" s="11004">
         <v>372</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="10519" t="s">
+      <c r="C10" s="10942" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="10528" t="s">
+      <c r="D10" s="10951" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="10537" t="s">
-        <v>192</v>
-      </c>
-      <c r="F10" s="10546" t="s">
+      <c r="E10" s="10960" t="s">
+        <v>212</v>
+      </c>
+      <c r="F10" s="10969" t="s">
         <v>213</v>
       </c>
       <c r="G10" s="9286"/>
-      <c r="H10" s="10555" t="s">
+      <c r="H10" s="10978" t="s">
         <v>214</v>
       </c>
-      <c r="I10" s="10564" t="s">
-        <v>195</v>
-      </c>
-      <c r="J10" s="10573" t="s">
-        <v>196</v>
+      <c r="I10" s="10987" t="s">
+        <v>215</v>
+      </c>
+      <c r="J10" s="10996" t="s">
+        <v>216</v>
       </c>
       <c r="K10"/>
-      <c r="L10" t="s" s="10582">
+      <c r="L10" t="s" s="11005">
         <v>373</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="10520" t="s">
+      <c r="C11" s="10943" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="10529" t="s">
+      <c r="D11" s="10952" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="10538" t="s">
-        <v>197</v>
-      </c>
-      <c r="F11" s="10547" t="s">
+      <c r="E11" s="10961" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" s="10970" t="s">
         <v>218</v>
       </c>
       <c r="G11" s="9287"/>
-      <c r="H11" s="10556" t="s">
+      <c r="H11" s="10979" t="s">
         <v>219</v>
       </c>
-      <c r="I11" s="10565" t="s">
-        <v>200</v>
-      </c>
-      <c r="J11" s="10574" t="s">
-        <v>201</v>
+      <c r="I11" s="10988" t="s">
+        <v>220</v>
+      </c>
+      <c r="J11" s="10997" t="s">
+        <v>221</v>
       </c>
       <c r="K11"/>
-      <c r="L11" t="s" s="10583">
+      <c r="L11" t="s" s="11006">
         <v>374</v>
       </c>
     </row>
@@ -45238,32 +46507,32 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="10584" t="s">
+      <c r="C3" s="11007" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="10590" t="s">
+      <c r="D3" s="11013" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="10596" t="s">
+      <c r="E3" s="11019" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="10602" t="s">
+      <c r="F3" s="11025" t="s">
         <v>224</v>
       </c>
-      <c r="G3" s="10608" t="s">
+      <c r="G3" s="11031" t="s">
         <v>225</v>
       </c>
-      <c r="H3" s="10614" t="s">
+      <c r="H3" s="11037" t="s">
         <v>375</v>
       </c>
       <c r="I3" s="9351"/>
-      <c r="J3" s="10620" t="s">
+      <c r="J3" s="11043" t="s">
         <v>381</v>
       </c>
-      <c r="K3" s="10626" t="s">
+      <c r="K3" s="11049" t="s">
         <v>228</v>
       </c>
-      <c r="L3" t="s" s="10632">
+      <c r="L3" t="s" s="11055">
         <v>387</v>
       </c>
       <c r="U3" s="9"/>
@@ -45279,32 +46548,32 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="10585" t="s">
+      <c r="C4" s="11008" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="10591" t="s">
+      <c r="D4" s="11014" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="10597" t="s">
+      <c r="E4" s="11020" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="10603" t="s">
+      <c r="F4" s="11026" t="s">
         <v>229</v>
       </c>
-      <c r="G4" s="10609" t="s">
+      <c r="G4" s="11032" t="s">
         <v>230</v>
       </c>
-      <c r="H4" s="10615" t="s">
+      <c r="H4" s="11038" t="s">
         <v>376</v>
       </c>
       <c r="I4" s="9352"/>
-      <c r="J4" s="10621" t="s">
+      <c r="J4" s="11044" t="s">
         <v>382</v>
       </c>
-      <c r="K4" s="10627" t="s">
+      <c r="K4" s="11050" t="s">
         <v>233</v>
       </c>
-      <c r="L4" t="s" s="10633">
+      <c r="L4" t="s" s="11056">
         <v>388</v>
       </c>
       <c r="U4" s="9"/>
@@ -45320,32 +46589,32 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="10586" t="s">
+      <c r="C5" s="11009" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="10592" t="s">
+      <c r="D5" s="11015" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="10598" t="s">
+      <c r="E5" s="11021" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="10604" t="s">
+      <c r="F5" s="11027" t="s">
         <v>224</v>
       </c>
-      <c r="G5" s="10610" t="s">
-        <v>239</v>
-      </c>
-      <c r="H5" s="10616" t="s">
+      <c r="G5" s="11033" t="s">
+        <v>234</v>
+      </c>
+      <c r="H5" s="11039" t="s">
         <v>377</v>
       </c>
       <c r="I5" s="9353"/>
-      <c r="J5" s="10622" t="s">
+      <c r="J5" s="11045" t="s">
         <v>383</v>
       </c>
-      <c r="K5" s="10628" t="s">
-        <v>242</v>
-      </c>
-      <c r="L5" t="s" s="10634">
+      <c r="K5" s="11051" t="s">
+        <v>228</v>
+      </c>
+      <c r="L5" t="s" s="11057">
         <v>389</v>
       </c>
       <c r="U5" s="9"/>
@@ -45361,32 +46630,32 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="10587" t="s">
+      <c r="C6" s="11010" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="10593" t="s">
+      <c r="D6" s="11016" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="10599" t="s">
+      <c r="E6" s="11022" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="10605" t="s">
+      <c r="F6" s="11028" t="s">
         <v>229</v>
       </c>
-      <c r="G6" s="10611" t="s">
+      <c r="G6" s="11034" t="s">
         <v>230</v>
       </c>
-      <c r="H6" s="10617" t="s">
+      <c r="H6" s="11040" t="s">
         <v>378</v>
       </c>
       <c r="I6" s="9354"/>
-      <c r="J6" s="10623" t="s">
+      <c r="J6" s="11046" t="s">
         <v>384</v>
       </c>
-      <c r="K6" s="10629" t="s">
+      <c r="K6" s="11052" t="s">
         <v>233</v>
       </c>
-      <c r="L6" t="s" s="10635">
+      <c r="L6" t="s" s="11058">
         <v>390</v>
       </c>
       <c r="U6" s="9"/>
@@ -45402,32 +46671,32 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="10588" t="s">
+      <c r="C7" s="11011" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="10594" t="s">
+      <c r="D7" s="11017" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="10600" t="s">
+      <c r="E7" s="11023" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="10606" t="s">
+      <c r="F7" s="11029" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="10612" t="s">
-        <v>234</v>
-      </c>
-      <c r="H7" s="10618" t="s">
+      <c r="G7" s="11035" t="s">
+        <v>239</v>
+      </c>
+      <c r="H7" s="11041" t="s">
         <v>379</v>
       </c>
       <c r="I7" s="9355"/>
-      <c r="J7" s="10624" t="s">
+      <c r="J7" s="11047" t="s">
         <v>385</v>
       </c>
-      <c r="K7" s="10630" t="s">
-        <v>228</v>
-      </c>
-      <c r="L7" t="s" s="10636">
+      <c r="K7" s="11053" t="s">
+        <v>242</v>
+      </c>
+      <c r="L7" t="s" s="11059">
         <v>391</v>
       </c>
       <c r="U7" s="9"/>
@@ -45443,32 +46712,32 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="10589" t="s">
+      <c r="C8" s="11012" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="10595" t="s">
+      <c r="D8" s="11018" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="10601" t="s">
+      <c r="E8" s="11024" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="10607" t="s">
+      <c r="F8" s="11030" t="s">
         <v>229</v>
       </c>
-      <c r="G8" s="10613" t="s">
+      <c r="G8" s="11036" t="s">
         <v>230</v>
       </c>
-      <c r="H8" s="10619" t="s">
+      <c r="H8" s="11042" t="s">
         <v>380</v>
       </c>
       <c r="I8" s="9356"/>
-      <c r="J8" s="10625" t="s">
+      <c r="J8" s="11048" t="s">
         <v>386</v>
       </c>
-      <c r="K8" s="10631" t="s">
+      <c r="K8" s="11054" t="s">
         <v>233</v>
       </c>
-      <c r="L8" t="s" s="10637">
+      <c r="L8" t="s" s="11060">
         <v>392</v>
       </c>
       <c r="U8" s="9"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-07-26 18:39:02] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Edu/Lessons/assumptionsMatter_femalesSing_math/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4553E54F-7F92-2543-A5C1-D67679C867EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56A1477-C87C-544A-ACF4-143297CDC7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33180" yWindow="1260" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,6 +62,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>5-6, 7-8, 9-12, etc. Leave blank if NA
 ======</t>
@@ -85,6 +86,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZoY
@@ -100,6 +102,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZoo
@@ -115,6 +118,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZoA
@@ -130,6 +134,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZow
@@ -145,6 +150,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZog
@@ -175,6 +181,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZos
@@ -190,6 +197,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZoU
@@ -205,6 +213,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZn4
@@ -220,6 +229,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZoM
@@ -235,6 +245,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZoQ
@@ -250,6 +261,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZoI
@@ -265,6 +277,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">======
 </t>
@@ -274,6 +287,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">ID#AAAAIbMHZn8
 </t>
@@ -283,6 +297,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">    (2021-05-10 01:43:14)
 </t>
@@ -292,6 +307,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>cloudinary or other CDN link for fast download</t>
         </r>
@@ -319,6 +335,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZoE
@@ -334,6 +351,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAAIbMHZoc
@@ -352,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="378">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1502,7 +1520,7 @@
     <t>(Optional) TEACHER Handout for Table 2 (P3)</t>
   </si>
   <si>
-    <t>https://catalog.galacticpolymath.com/Lessons/assumptionsMatter_femalesSing_math/Sing_P3_Table 2_TEACHER.docx</t>
+    <t>https://catalog.galacticpolymath.com/lessons/assumptionsmatter_femalessing_math/Females%20Sing_P3_Table%202_TEACHER.docx</t>
   </si>
 </sst>
 </file>
@@ -1521,39 +1539,41 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1564,90 +1584,98 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <b/>
@@ -1660,28 +1688,32 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Roboto mono"/>
+      <name val="Roboto Mono"/>
     </font>
     <font>
       <b/>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1827,7 +1859,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1376">
+  <cellXfs count="957">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2068,6 +2100,26 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
@@ -3335,1281 +3387,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -6198,13 +4975,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="519" t="s">
+      <c r="A1" s="527" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="520"/>
-      <c r="C1" s="520"/>
-      <c r="D1" s="520"/>
-      <c r="E1" s="521"/>
+      <c r="B1" s="528"/>
+      <c r="C1" s="528"/>
+      <c r="D1" s="528"/>
+      <c r="E1" s="529"/>
     </row>
     <row r="2" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -13669,14 +12446,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="522" t="s">
+      <c r="A1" s="530" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="520"/>
-      <c r="C1" s="520"/>
-      <c r="D1" s="520"/>
-      <c r="E1" s="520"/>
-      <c r="F1" s="521"/>
+      <c r="B1" s="528"/>
+      <c r="C1" s="528"/>
+      <c r="D1" s="528"/>
+      <c r="E1" s="528"/>
+      <c r="F1" s="529"/>
     </row>
     <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -13720,170 +12497,170 @@
       <c r="AA2" s="4"/>
     </row>
     <row r="3" spans="1:27" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="953" t="s">
+      <c r="A3" s="534" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="961" t="s">
+      <c r="B3" s="542" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="969" t="s">
+      <c r="C3" s="550" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="977" t="s">
+      <c r="D3" s="558" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="985" t="s">
+      <c r="E3" s="566" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="49"/>
-      <c r="G3" s="993" t="s">
+      <c r="G3" s="574" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="954" t="s">
+      <c r="A4" s="535" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="962" t="s">
+      <c r="B4" s="543" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="970" t="s">
+      <c r="C4" s="551" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="978" t="s">
+      <c r="D4" s="559" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="986" t="s">
+      <c r="E4" s="567" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="50"/>
-      <c r="G4" s="994" t="s">
+      <c r="G4" s="575" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="70" x14ac:dyDescent="0.15">
-      <c r="A5" s="955" t="s">
+      <c r="A5" s="536" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="963" t="s">
+      <c r="B5" s="544" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="971" t="s">
+      <c r="C5" s="552" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="979" t="s">
+      <c r="D5" s="560" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="987" t="s">
+      <c r="E5" s="568" t="s">
         <v>45</v>
       </c>
       <c r="F5" s="51"/>
-      <c r="G5" s="995" t="s">
+      <c r="G5" s="576" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="56" x14ac:dyDescent="0.15">
-      <c r="A6" s="956" t="s">
+      <c r="A6" s="537" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="964" t="s">
+      <c r="B6" s="545" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="972" t="s">
+      <c r="C6" s="553" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="980" t="s">
+      <c r="D6" s="561" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="988" t="s">
+      <c r="E6" s="569" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="52"/>
-      <c r="G6" s="996" t="s">
+      <c r="G6" s="577" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="56" x14ac:dyDescent="0.15">
-      <c r="A7" s="957" t="s">
+      <c r="A7" s="538" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="965" t="s">
+      <c r="B7" s="546" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="973" t="s">
+      <c r="C7" s="554" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="981" t="s">
+      <c r="D7" s="562" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="989" t="s">
+      <c r="E7" s="570" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="53"/>
-      <c r="G7" s="997" t="s">
+      <c r="G7" s="578" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="56" x14ac:dyDescent="0.15">
-      <c r="A8" s="958" t="s">
+      <c r="A8" s="539" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="966" t="s">
+      <c r="B8" s="547" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="974" t="s">
+      <c r="C8" s="555" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="982" t="s">
+      <c r="D8" s="563" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="990" t="s">
+      <c r="E8" s="571" t="s">
         <v>51</v>
       </c>
       <c r="F8" s="54"/>
-      <c r="G8" s="998" t="s">
+      <c r="G8" s="579" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="56" x14ac:dyDescent="0.15">
-      <c r="A9" s="959" t="s">
+      <c r="A9" s="540" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="967" t="s">
+      <c r="B9" s="548" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="975" t="s">
+      <c r="C9" s="556" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="983" t="s">
+      <c r="D9" s="564" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="991" t="s">
+      <c r="E9" s="572" t="s">
         <v>53</v>
       </c>
       <c r="F9" s="55"/>
-      <c r="G9" s="999" t="s">
+      <c r="G9" s="580" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="56" x14ac:dyDescent="0.15">
-      <c r="A10" s="960" t="s">
+      <c r="A10" s="541" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="968" t="s">
+      <c r="B10" s="549" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="976" t="s">
+      <c r="C10" s="557" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="984" t="s">
+      <c r="D10" s="565" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="992" t="s">
+      <c r="E10" s="573" t="s">
         <v>55</v>
       </c>
       <c r="F10" s="56"/>
-      <c r="G10" s="1000" t="s">
+      <c r="G10" s="581" t="s">
         <v>291</v>
       </c>
     </row>
@@ -13936,19 +12713,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="523" t="s">
+      <c r="A1" s="531" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="520"/>
-      <c r="C1" s="520"/>
-      <c r="D1" s="520"/>
-      <c r="E1" s="520"/>
-      <c r="F1" s="520"/>
-      <c r="G1" s="520"/>
-      <c r="H1" s="520"/>
-      <c r="I1" s="520"/>
-      <c r="J1" s="520"/>
-      <c r="K1" s="521"/>
+      <c r="B1" s="528"/>
+      <c r="C1" s="528"/>
+      <c r="D1" s="528"/>
+      <c r="E1" s="528"/>
+      <c r="F1" s="528"/>
+      <c r="G1" s="528"/>
+      <c r="H1" s="528"/>
+      <c r="I1" s="528"/>
+      <c r="J1" s="528"/>
+      <c r="K1" s="529"/>
       <c r="L1" s="12"/>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
@@ -14008,243 +12785,243 @@
     <row r="3" spans="1:32" ht="112" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="1001" t="s">
+      <c r="C3" s="582" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1010" t="s">
+      <c r="D3" s="591" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="1019" t="s">
+      <c r="E3" s="600" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="1028" t="s">
+      <c r="F3" s="609" t="s">
         <v>65</v>
       </c>
       <c r="G3" s="57"/>
-      <c r="H3" s="1037" t="s">
+      <c r="H3" s="618" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="1046" t="s">
+      <c r="I3" s="627" t="s">
         <v>67</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="1055" t="s">
+      <c r="K3" s="636" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="112" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="1002" t="s">
+      <c r="C4" s="583" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="1011" t="s">
+      <c r="D4" s="592" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="1020" t="s">
+      <c r="E4" s="601" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="1029" t="s">
+      <c r="F4" s="610" t="s">
         <v>70</v>
       </c>
       <c r="G4" s="58"/>
-      <c r="H4" s="1038" t="s">
+      <c r="H4" s="619" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="1047" t="s">
+      <c r="I4" s="628" t="s">
         <v>72</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1056" t="s">
+      <c r="K4" s="637" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="112" x14ac:dyDescent="0.15">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="1003" t="s">
+      <c r="C5" s="584" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="1012" t="s">
+      <c r="D5" s="593" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="1021" t="s">
+      <c r="E5" s="602" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="1030" t="s">
+      <c r="F5" s="611" t="s">
         <v>75</v>
       </c>
       <c r="G5" s="59"/>
-      <c r="H5" s="1039" t="s">
+      <c r="H5" s="620" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="1048" t="s">
+      <c r="I5" s="629" t="s">
         <v>77</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1057" t="s">
+      <c r="K5" s="638" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="126" x14ac:dyDescent="0.15">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="1004" t="s">
+      <c r="C6" s="585" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="1013" t="s">
+      <c r="D6" s="594" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="1022" t="s">
+      <c r="E6" s="603" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="1031" t="s">
+      <c r="F6" s="612" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="60"/>
-      <c r="H6" s="1040" t="s">
+      <c r="H6" s="621" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="1049" t="s">
+      <c r="I6" s="630" t="s">
         <v>81</v>
       </c>
       <c r="J6"/>
-      <c r="K6" s="1058" t="s">
+      <c r="K6" s="639" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="112" x14ac:dyDescent="0.15">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="1005" t="s">
+      <c r="C7" s="586" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="1014" t="s">
+      <c r="D7" s="595" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="1023" t="s">
+      <c r="E7" s="604" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="1032" t="s">
+      <c r="F7" s="613" t="s">
         <v>83</v>
       </c>
       <c r="G7" s="61"/>
-      <c r="H7" s="1041" t="s">
+      <c r="H7" s="622" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="1050" t="s">
+      <c r="I7" s="631" t="s">
         <v>85</v>
       </c>
       <c r="J7"/>
-      <c r="K7" s="1059" t="s">
+      <c r="K7" s="640" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="112" x14ac:dyDescent="0.15">
       <c r="A8" s="19"/>
       <c r="B8"/>
-      <c r="C8" s="1006" t="s">
+      <c r="C8" s="587" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="1015" t="s">
+      <c r="D8" s="596" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="1024" t="s">
+      <c r="E8" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="1033" t="s">
+      <c r="F8" s="614" t="s">
         <v>87</v>
       </c>
       <c r="G8" s="62"/>
-      <c r="H8" s="1042" t="s">
+      <c r="H8" s="623" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="1051" t="s">
+      <c r="I8" s="632" t="s">
         <v>89</v>
       </c>
       <c r="J8"/>
-      <c r="K8" s="1060" t="s">
+      <c r="K8" s="641" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="112" x14ac:dyDescent="0.15">
       <c r="A9" s="19"/>
       <c r="B9"/>
-      <c r="C9" s="1007" t="s">
+      <c r="C9" s="588" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="1016" t="s">
+      <c r="D9" s="597" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="1025" t="s">
+      <c r="E9" s="606" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="1034" t="s">
+      <c r="F9" s="615" t="s">
         <v>91</v>
       </c>
       <c r="G9" s="63"/>
-      <c r="H9" s="1043" t="s">
+      <c r="H9" s="624" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="1052" t="s">
+      <c r="I9" s="633" t="s">
         <v>93</v>
       </c>
       <c r="J9"/>
-      <c r="K9" s="1061" t="s">
+      <c r="K9" s="642" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="112" x14ac:dyDescent="0.15">
       <c r="A10" s="19"/>
       <c r="B10"/>
-      <c r="C10" s="1008" t="s">
+      <c r="C10" s="589" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="1017" t="s">
+      <c r="D10" s="598" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="1026" t="s">
+      <c r="E10" s="607" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="1035" t="s">
+      <c r="F10" s="616" t="s">
         <v>95</v>
       </c>
       <c r="G10" s="64"/>
-      <c r="H10" s="1044" t="s">
+      <c r="H10" s="625" t="s">
         <v>96</v>
       </c>
-      <c r="I10" s="1053" t="s">
+      <c r="I10" s="634" t="s">
         <v>97</v>
       </c>
       <c r="J10"/>
-      <c r="K10" s="1062" t="s">
+      <c r="K10" s="643" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="126" x14ac:dyDescent="0.15">
       <c r="A11" s="19"/>
       <c r="B11"/>
-      <c r="C11" s="1009" t="s">
+      <c r="C11" s="590" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="1018" t="s">
+      <c r="D11" s="599" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="1027" t="s">
+      <c r="E11" s="608" t="s">
         <v>98</v>
       </c>
-      <c r="F11" s="1036" t="s">
+      <c r="F11" s="617" t="s">
         <v>99</v>
       </c>
       <c r="G11" s="65"/>
-      <c r="H11" s="1045" t="s">
+      <c r="H11" s="626" t="s">
         <v>100</v>
       </c>
-      <c r="I11" s="1054" t="s">
+      <c r="I11" s="635" t="s">
         <v>101</v>
       </c>
       <c r="J11"/>
-      <c r="K11" s="1063" t="s">
+      <c r="K11" s="644" t="s">
         <v>300</v>
       </c>
     </row>
@@ -14742,19 +13519,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="523" t="s">
+      <c r="A1" s="531" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="520"/>
-      <c r="C1" s="520"/>
-      <c r="D1" s="520"/>
-      <c r="E1" s="520"/>
-      <c r="F1" s="520"/>
-      <c r="G1" s="520"/>
-      <c r="H1" s="520"/>
-      <c r="I1" s="520"/>
-      <c r="J1" s="520"/>
-      <c r="K1" s="521"/>
+      <c r="B1" s="528"/>
+      <c r="C1" s="528"/>
+      <c r="D1" s="528"/>
+      <c r="E1" s="528"/>
+      <c r="F1" s="528"/>
+      <c r="G1" s="528"/>
+      <c r="H1" s="528"/>
+      <c r="I1" s="528"/>
+      <c r="J1" s="528"/>
+      <c r="K1" s="529"/>
       <c r="L1" s="20"/>
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
@@ -14834,32 +13611,32 @@
     <row r="3" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="1064" t="s">
+      <c r="C3" s="645" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1085" t="s">
+      <c r="D3" s="666" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="1106" t="s">
+      <c r="E3" s="687" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="1124" t="s">
+      <c r="F3" s="705" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1145" t="s">
+      <c r="G3" s="726" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="1166" t="s">
+      <c r="H3" s="747" t="s">
         <v>108</v>
       </c>
       <c r="I3" s="66"/>
-      <c r="J3" s="1187" t="s">
+      <c r="J3" s="768" t="s">
         <v>346</v>
       </c>
-      <c r="K3" s="1208" t="s">
+      <c r="K3" s="789" t="s">
         <v>109</v>
       </c>
-      <c r="L3" s="1229" t="s">
+      <c r="L3" s="810" t="s">
         <v>304</v>
       </c>
       <c r="U3" s="6"/>
@@ -14873,32 +13650,32 @@
     <row r="4" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="1065" t="s">
+      <c r="C4" s="646" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="1086" t="s">
+      <c r="D4" s="667" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="1107" t="s">
+      <c r="E4" s="688" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="1125" t="s">
+      <c r="F4" s="706" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1146" t="s">
+      <c r="G4" s="727" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="1167" t="s">
+      <c r="H4" s="748" t="s">
         <v>112</v>
       </c>
       <c r="I4" s="67"/>
-      <c r="J4" s="1188" t="s">
+      <c r="J4" s="769" t="s">
         <v>347</v>
       </c>
-      <c r="K4" s="1209" t="s">
+      <c r="K4" s="790" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="1230" t="s">
+      <c r="L4" s="811" t="s">
         <v>305</v>
       </c>
       <c r="U4" s="6"/>
@@ -14912,32 +13689,32 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="1066" t="s">
+      <c r="C5" s="647" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="1087" t="s">
+      <c r="D5" s="668" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="1108" t="s">
+      <c r="E5" s="689" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="1126" t="s">
+      <c r="F5" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="1147" t="s">
+      <c r="G5" s="728" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="1168" t="s">
+      <c r="H5" s="749" t="s">
         <v>115</v>
       </c>
       <c r="I5" s="68"/>
-      <c r="J5" s="1189" t="s">
+      <c r="J5" s="770" t="s">
         <v>348</v>
       </c>
-      <c r="K5" s="1210" t="s">
+      <c r="K5" s="791" t="s">
         <v>116</v>
       </c>
-      <c r="L5" s="1231" t="s">
+      <c r="L5" s="812" t="s">
         <v>306</v>
       </c>
       <c r="U5" s="6"/>
@@ -14951,32 +13728,32 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="1067" t="s">
+      <c r="C6" s="648" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="1088" t="s">
+      <c r="D6" s="669" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="1109" t="s">
+      <c r="E6" s="690" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="1127" t="s">
+      <c r="F6" s="708" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="1148" t="s">
+      <c r="G6" s="729" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="1169" t="s">
+      <c r="H6" s="750" t="s">
         <v>118</v>
       </c>
       <c r="I6" s="69"/>
-      <c r="J6" s="1190" t="s">
+      <c r="J6" s="771" t="s">
         <v>349</v>
       </c>
-      <c r="K6" s="1211" t="s">
+      <c r="K6" s="792" t="s">
         <v>119</v>
       </c>
-      <c r="L6" s="1232" t="s">
+      <c r="L6" s="813" t="s">
         <v>307</v>
       </c>
       <c r="U6" s="6"/>
@@ -14990,32 +13767,32 @@
     <row r="7" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="1068" t="s">
+      <c r="C7" s="649" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="1089" t="s">
+      <c r="D7" s="670" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="1110" t="s">
+      <c r="E7" s="691" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="1128" t="s">
+      <c r="F7" s="709" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1149" t="s">
+      <c r="G7" s="730" t="s">
         <v>120</v>
       </c>
-      <c r="H7" s="1170" t="s">
+      <c r="H7" s="751" t="s">
         <v>121</v>
       </c>
       <c r="I7" s="70"/>
-      <c r="J7" s="1191" t="s">
+      <c r="J7" s="772" t="s">
         <v>350</v>
       </c>
-      <c r="K7" s="1212" t="s">
+      <c r="K7" s="793" t="s">
         <v>122</v>
       </c>
-      <c r="L7" s="1233" t="s">
+      <c r="L7" s="814" t="s">
         <v>308</v>
       </c>
       <c r="U7" s="6"/>
@@ -15029,32 +13806,32 @@
     <row r="8" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8"/>
-      <c r="C8" s="1069" t="s">
+      <c r="C8" s="650" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="1090" t="s">
+      <c r="D8" s="671" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="1111" t="s">
+      <c r="E8" s="692" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="1129" t="s">
+      <c r="F8" s="710" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="1150" t="s">
+      <c r="G8" s="731" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="1171" t="s">
+      <c r="H8" s="752" t="s">
         <v>124</v>
       </c>
       <c r="I8" s="71"/>
-      <c r="J8" s="1192" t="s">
+      <c r="J8" s="773" t="s">
         <v>351</v>
       </c>
-      <c r="K8" s="1213" t="s">
+      <c r="K8" s="794" t="s">
         <v>125</v>
       </c>
-      <c r="L8" s="1234" t="s">
+      <c r="L8" s="815" t="s">
         <v>309</v>
       </c>
       <c r="U8" s="6"/>
@@ -15068,30 +13845,30 @@
     <row r="9" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9"/>
-      <c r="C9" s="1070" t="s">
+      <c r="C9" s="651" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="1091" t="s">
+      <c r="D9" s="672" t="s">
         <v>73</v>
       </c>
       <c r="E9" s="19"/>
-      <c r="F9" s="1130" t="s">
+      <c r="F9" s="711" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="1151" t="s">
+      <c r="G9" s="732" t="s">
         <v>127</v>
       </c>
-      <c r="H9" s="1172" t="s">
+      <c r="H9" s="753" t="s">
         <v>128</v>
       </c>
       <c r="I9" s="72"/>
-      <c r="J9" s="1193" t="s">
+      <c r="J9" s="774" t="s">
         <v>352</v>
       </c>
-      <c r="K9" s="1214" t="s">
+      <c r="K9" s="795" t="s">
         <v>301</v>
       </c>
-      <c r="L9" s="1235" t="s">
+      <c r="L9" s="816" t="s">
         <v>310</v>
       </c>
       <c r="U9" s="6"/>
@@ -15105,32 +13882,32 @@
     <row r="10" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10"/>
-      <c r="C10" s="1071" t="s">
+      <c r="C10" s="652" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="1092" t="s">
+      <c r="D10" s="673" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="1112" t="s">
+      <c r="E10" s="693" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="1131" t="s">
+      <c r="F10" s="712" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="1152" t="s">
+      <c r="G10" s="733" t="s">
         <v>129</v>
       </c>
-      <c r="H10" s="1173" t="s">
+      <c r="H10" s="754" t="s">
         <v>130</v>
       </c>
       <c r="I10" s="73"/>
-      <c r="J10" s="1194" t="s">
+      <c r="J10" s="775" t="s">
         <v>353</v>
       </c>
-      <c r="K10" s="1215" t="s">
+      <c r="K10" s="796" t="s">
         <v>131</v>
       </c>
-      <c r="L10" s="1236" t="s">
+      <c r="L10" s="817" t="s">
         <v>311</v>
       </c>
       <c r="U10" s="6"/>
@@ -15144,32 +13921,32 @@
     <row r="11" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11"/>
-      <c r="C11" s="1072" t="s">
+      <c r="C11" s="653" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1093" t="s">
+      <c r="D11" s="674" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="1113" t="s">
+      <c r="E11" s="694" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="1132" t="s">
+      <c r="F11" s="713" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="1153" t="s">
+      <c r="G11" s="734" t="s">
         <v>132</v>
       </c>
-      <c r="H11" s="1174" t="s">
+      <c r="H11" s="755" t="s">
         <v>133</v>
       </c>
       <c r="I11" s="74"/>
-      <c r="J11" s="1195" t="s">
+      <c r="J11" s="776" t="s">
         <v>354</v>
       </c>
-      <c r="K11" s="1216" t="s">
+      <c r="K11" s="797" t="s">
         <v>134</v>
       </c>
-      <c r="L11" s="1237" t="s">
+      <c r="L11" s="818" t="s">
         <v>312</v>
       </c>
       <c r="U11" s="6"/>
@@ -15183,32 +13960,32 @@
     <row r="12" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12"/>
-      <c r="C12" s="1073" t="s">
+      <c r="C12" s="654" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="1094" t="s">
+      <c r="D12" s="675" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="1114" t="s">
+      <c r="E12" s="695" t="s">
         <v>106</v>
       </c>
-      <c r="F12" s="1133" t="s">
+      <c r="F12" s="714" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="1154" t="s">
+      <c r="G12" s="735" t="s">
         <v>135</v>
       </c>
-      <c r="H12" s="1175" t="s">
+      <c r="H12" s="756" t="s">
         <v>136</v>
       </c>
       <c r="I12" s="75"/>
-      <c r="J12" s="1196" t="s">
+      <c r="J12" s="777" t="s">
         <v>355</v>
       </c>
-      <c r="K12" s="1217" t="s">
+      <c r="K12" s="798" t="s">
         <v>137</v>
       </c>
-      <c r="L12" s="1238" t="s">
+      <c r="L12" s="819" t="s">
         <v>313</v>
       </c>
       <c r="U12" s="6"/>
@@ -15222,32 +13999,32 @@
     <row r="13" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13"/>
-      <c r="C13" s="1074" t="s">
+      <c r="C13" s="655" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="1095" t="s">
+      <c r="D13" s="676" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="1115" t="s">
+      <c r="E13" s="696" t="s">
         <v>110</v>
       </c>
-      <c r="F13" s="1134" t="s">
+      <c r="F13" s="715" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="1155" t="s">
+      <c r="G13" s="736" t="s">
         <v>138</v>
       </c>
-      <c r="H13" s="1176" t="s">
+      <c r="H13" s="757" t="s">
         <v>139</v>
       </c>
       <c r="I13" s="76"/>
-      <c r="J13" s="1197" t="s">
+      <c r="J13" s="778" t="s">
         <v>356</v>
       </c>
-      <c r="K13" s="1218" t="s">
+      <c r="K13" s="799" t="s">
         <v>140</v>
       </c>
-      <c r="L13" s="1239" t="s">
+      <c r="L13" s="820" t="s">
         <v>314</v>
       </c>
       <c r="U13" s="6"/>
@@ -15261,32 +14038,32 @@
     <row r="14" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14"/>
-      <c r="C14" s="1075" t="s">
+      <c r="C14" s="656" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="1096" t="s">
+      <c r="D14" s="677" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="1116" t="s">
+      <c r="E14" s="697" t="s">
         <v>106</v>
       </c>
-      <c r="F14" s="1135" t="s">
+      <c r="F14" s="716" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="1156" t="s">
+      <c r="G14" s="737" t="s">
         <v>141</v>
       </c>
-      <c r="H14" s="1177" t="s">
+      <c r="H14" s="758" t="s">
         <v>142</v>
       </c>
       <c r="I14" s="77"/>
-      <c r="J14" s="1198" t="s">
+      <c r="J14" s="779" t="s">
         <v>357</v>
       </c>
-      <c r="K14" s="1219" t="s">
+      <c r="K14" s="800" t="s">
         <v>143</v>
       </c>
-      <c r="L14" s="1240" t="s">
+      <c r="L14" s="821" t="s">
         <v>315</v>
       </c>
       <c r="U14" s="6"/>
@@ -15300,32 +14077,32 @@
     <row r="15" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15"/>
-      <c r="C15" s="1076" t="s">
+      <c r="C15" s="657" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="1097" t="s">
+      <c r="D15" s="678" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="1117" t="s">
+      <c r="E15" s="698" t="s">
         <v>110</v>
       </c>
-      <c r="F15" s="1136" t="s">
+      <c r="F15" s="717" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="1157" t="s">
+      <c r="G15" s="738" t="s">
         <v>144</v>
       </c>
-      <c r="H15" s="1178" t="s">
+      <c r="H15" s="759" t="s">
         <v>145</v>
       </c>
       <c r="I15" s="78"/>
-      <c r="J15" s="1199" t="s">
+      <c r="J15" s="780" t="s">
         <v>358</v>
       </c>
-      <c r="K15" s="1220" t="s">
+      <c r="K15" s="801" t="s">
         <v>146</v>
       </c>
-      <c r="L15" s="1241" t="s">
+      <c r="L15" s="822" t="s">
         <v>316</v>
       </c>
       <c r="U15" s="6"/>
@@ -15339,30 +14116,30 @@
     <row r="16" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16"/>
-      <c r="C16" s="1077" t="s">
+      <c r="C16" s="658" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="1098" t="s">
+      <c r="D16" s="679" t="s">
         <v>73</v>
       </c>
       <c r="E16" s="19"/>
-      <c r="F16" s="1137" t="s">
+      <c r="F16" s="718" t="s">
         <v>126</v>
       </c>
-      <c r="G16" s="1158" t="s">
+      <c r="G16" s="739" t="s">
         <v>147</v>
       </c>
-      <c r="H16" s="1179" t="s">
+      <c r="H16" s="760" t="s">
         <v>148</v>
       </c>
       <c r="I16" s="79"/>
-      <c r="J16" s="1200" t="s">
+      <c r="J16" s="781" t="s">
         <v>359</v>
       </c>
-      <c r="K16" s="1221" t="s">
+      <c r="K16" s="802" t="s">
         <v>302</v>
       </c>
-      <c r="L16" s="1242" t="s">
+      <c r="L16" s="823" t="s">
         <v>317</v>
       </c>
       <c r="U16" s="6"/>
@@ -15376,32 +14153,32 @@
     <row r="17" spans="1:27" ht="100" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17"/>
-      <c r="C17" s="1078" t="s">
+      <c r="C17" s="659" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="1099" t="s">
+      <c r="D17" s="680" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="1118" t="s">
+      <c r="E17" s="699" t="s">
         <v>106</v>
       </c>
-      <c r="F17" s="1138" t="s">
+      <c r="F17" s="719" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="1159" t="s">
+      <c r="G17" s="740" t="s">
         <v>149</v>
       </c>
-      <c r="H17" s="1180" t="s">
+      <c r="H17" s="761" t="s">
         <v>150</v>
       </c>
       <c r="I17" s="80"/>
-      <c r="J17" s="1201" t="s">
+      <c r="J17" s="782" t="s">
         <v>360</v>
       </c>
-      <c r="K17" s="1222" t="s">
+      <c r="K17" s="803" t="s">
         <v>151</v>
       </c>
-      <c r="L17" s="1243" t="s">
+      <c r="L17" s="824" t="s">
         <v>318</v>
       </c>
       <c r="U17" s="6"/>
@@ -15415,32 +14192,32 @@
     <row r="18" spans="1:27" ht="86" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18"/>
-      <c r="C18" s="1079" t="s">
+      <c r="C18" s="660" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="1100" t="s">
+      <c r="D18" s="681" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="1119" t="s">
+      <c r="E18" s="700" t="s">
         <v>110</v>
       </c>
-      <c r="F18" s="1139" t="s">
+      <c r="F18" s="720" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="1160" t="s">
+      <c r="G18" s="741" t="s">
         <v>152</v>
       </c>
-      <c r="H18" s="1181" t="s">
+      <c r="H18" s="762" t="s">
         <v>153</v>
       </c>
       <c r="I18" s="81"/>
-      <c r="J18" s="1202" t="s">
+      <c r="J18" s="783" t="s">
         <v>361</v>
       </c>
-      <c r="K18" s="1223" t="s">
+      <c r="K18" s="804" t="s">
         <v>154</v>
       </c>
-      <c r="L18" s="1244" t="s">
+      <c r="L18" s="825" t="s">
         <v>319</v>
       </c>
       <c r="U18" s="6"/>
@@ -15454,32 +14231,32 @@
     <row r="19" spans="1:27" ht="100" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19"/>
-      <c r="C19" s="1080" t="s">
+      <c r="C19" s="661" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="1101" t="s">
+      <c r="D19" s="682" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="1120" t="s">
+      <c r="E19" s="701" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="1140" t="s">
+      <c r="F19" s="721" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="1161" t="s">
+      <c r="G19" s="742" t="s">
         <v>155</v>
       </c>
-      <c r="H19" s="1182" t="s">
+      <c r="H19" s="763" t="s">
         <v>156</v>
       </c>
       <c r="I19" s="82"/>
-      <c r="J19" s="1203" t="s">
+      <c r="J19" s="784" t="s">
         <v>362</v>
       </c>
-      <c r="K19" s="1224" t="s">
+      <c r="K19" s="805" t="s">
         <v>157</v>
       </c>
-      <c r="L19" s="1245" t="s">
+      <c r="L19" s="826" t="s">
         <v>320</v>
       </c>
       <c r="U19" s="6"/>
@@ -15493,32 +14270,32 @@
     <row r="20" spans="1:27" ht="100" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20"/>
-      <c r="C20" s="1081" t="s">
+      <c r="C20" s="662" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="1102" t="s">
+      <c r="D20" s="683" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="1121" t="s">
+      <c r="E20" s="702" t="s">
         <v>110</v>
       </c>
-      <c r="F20" s="1141" t="s">
+      <c r="F20" s="722" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="1162" t="s">
+      <c r="G20" s="743" t="s">
         <v>158</v>
       </c>
-      <c r="H20" s="1183" t="s">
+      <c r="H20" s="764" t="s">
         <v>159</v>
       </c>
       <c r="I20" s="83"/>
-      <c r="J20" s="1204" t="s">
+      <c r="J20" s="785" t="s">
         <v>363</v>
       </c>
-      <c r="K20" s="1225" t="s">
+      <c r="K20" s="806" t="s">
         <v>160</v>
       </c>
-      <c r="L20" s="1246" t="s">
+      <c r="L20" s="827" t="s">
         <v>321</v>
       </c>
       <c r="U20" s="6"/>
@@ -15532,32 +14309,32 @@
     <row r="21" spans="1:27" ht="100" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21"/>
-      <c r="C21" s="1082" t="s">
+      <c r="C21" s="663" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="1103" t="s">
+      <c r="D21" s="684" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="1122" t="s">
+      <c r="E21" s="703" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="1142" t="s">
+      <c r="F21" s="723" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="1163" t="s">
+      <c r="G21" s="744" t="s">
         <v>161</v>
       </c>
-      <c r="H21" s="1184" t="s">
+      <c r="H21" s="765" t="s">
         <v>162</v>
       </c>
       <c r="I21" s="84"/>
-      <c r="J21" s="1205" t="s">
+      <c r="J21" s="786" t="s">
         <v>364</v>
       </c>
-      <c r="K21" s="1226" t="s">
+      <c r="K21" s="807" t="s">
         <v>163</v>
       </c>
-      <c r="L21" s="1247" t="s">
+      <c r="L21" s="828" t="s">
         <v>322</v>
       </c>
       <c r="U21" s="6"/>
@@ -15571,32 +14348,32 @@
     <row r="22" spans="1:27" ht="100" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22"/>
-      <c r="C22" s="1083" t="s">
+      <c r="C22" s="664" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="1104" t="s">
+      <c r="D22" s="685" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="1123" t="s">
+      <c r="E22" s="704" t="s">
         <v>110</v>
       </c>
-      <c r="F22" s="1143" t="s">
+      <c r="F22" s="724" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="1164" t="s">
+      <c r="G22" s="745" t="s">
         <v>164</v>
       </c>
-      <c r="H22" s="1185" t="s">
+      <c r="H22" s="766" t="s">
         <v>165</v>
       </c>
       <c r="I22" s="85"/>
-      <c r="J22" s="1206" t="s">
+      <c r="J22" s="787" t="s">
         <v>365</v>
       </c>
-      <c r="K22" s="1227" t="s">
+      <c r="K22" s="808" t="s">
         <v>166</v>
       </c>
-      <c r="L22" s="1248" t="s">
+      <c r="L22" s="829" t="s">
         <v>323</v>
       </c>
       <c r="U22" s="6"/>
@@ -15610,30 +14387,30 @@
     <row r="23" spans="1:27" ht="100" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23"/>
-      <c r="C23" s="1084" t="s">
+      <c r="C23" s="665" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="1105" t="s">
+      <c r="D23" s="686" t="s">
         <v>73</v>
       </c>
       <c r="E23" s="19"/>
-      <c r="F23" s="1144" t="s">
+      <c r="F23" s="725" t="s">
         <v>126</v>
       </c>
-      <c r="G23" s="1165" t="s">
+      <c r="G23" s="746" t="s">
         <v>167</v>
       </c>
-      <c r="H23" s="1186" t="s">
+      <c r="H23" s="767" t="s">
         <v>168</v>
       </c>
       <c r="I23" s="86"/>
-      <c r="J23" s="1207" t="s">
+      <c r="J23" s="788" t="s">
         <v>366</v>
       </c>
-      <c r="K23" s="1228" t="s">
+      <c r="K23" s="809" t="s">
         <v>303</v>
       </c>
-      <c r="L23" s="1249" t="s">
+      <c r="L23" s="830" t="s">
         <v>324</v>
       </c>
       <c r="U23" s="6"/>
@@ -16540,19 +15317,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="524" t="s">
+      <c r="A1" s="532" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="520"/>
-      <c r="C1" s="520"/>
-      <c r="D1" s="520"/>
-      <c r="E1" s="520"/>
-      <c r="F1" s="520"/>
-      <c r="G1" s="520"/>
-      <c r="H1" s="520"/>
-      <c r="I1" s="520"/>
-      <c r="J1" s="520"/>
-      <c r="K1" s="521"/>
+      <c r="B1" s="528"/>
+      <c r="C1" s="528"/>
+      <c r="D1" s="528"/>
+      <c r="E1" s="528"/>
+      <c r="F1" s="528"/>
+      <c r="G1" s="528"/>
+      <c r="H1" s="528"/>
+      <c r="I1" s="528"/>
+      <c r="J1" s="528"/>
+      <c r="K1" s="529"/>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
     </row>
@@ -16616,270 +15393,270 @@
     <row r="3" spans="1:33" ht="84" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="1250" t="s">
+      <c r="C3" s="831" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1259" t="s">
+      <c r="D3" s="840" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="1268" t="s">
+      <c r="E3" s="849" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="1277" t="s">
+      <c r="F3" s="858" t="s">
         <v>173</v>
       </c>
       <c r="G3" s="87"/>
-      <c r="H3" s="1286" t="s">
+      <c r="H3" s="867" t="s">
         <v>174</v>
       </c>
-      <c r="I3" s="1295" t="s">
+      <c r="I3" s="876" t="s">
         <v>175</v>
       </c>
-      <c r="J3" s="1304" t="s">
+      <c r="J3" s="885" t="s">
         <v>176</v>
       </c>
       <c r="K3"/>
-      <c r="L3" s="1313" t="s">
+      <c r="L3" s="894" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="84" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="1251" t="s">
+      <c r="C4" s="832" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="1260" t="s">
+      <c r="D4" s="841" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="1269" t="s">
+      <c r="E4" s="850" t="s">
         <v>177</v>
       </c>
-      <c r="F4" s="1278" t="s">
+      <c r="F4" s="859" t="s">
         <v>178</v>
       </c>
       <c r="G4" s="88"/>
-      <c r="H4" s="1287" t="s">
+      <c r="H4" s="868" t="s">
         <v>179</v>
       </c>
-      <c r="I4" s="1296" t="s">
+      <c r="I4" s="877" t="s">
         <v>180</v>
       </c>
-      <c r="J4" s="1305" t="s">
+      <c r="J4" s="886" t="s">
         <v>181</v>
       </c>
       <c r="K4"/>
-      <c r="L4" s="1314" t="s">
+      <c r="L4" s="895" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="84" x14ac:dyDescent="0.15">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="1252" t="s">
+      <c r="C5" s="833" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="1261" t="s">
+      <c r="D5" s="842" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="1270" t="s">
+      <c r="E5" s="851" t="s">
         <v>182</v>
       </c>
-      <c r="F5" s="1279" t="s">
+      <c r="F5" s="860" t="s">
         <v>183</v>
       </c>
       <c r="G5" s="89"/>
-      <c r="H5" s="1288" t="s">
+      <c r="H5" s="869" t="s">
         <v>184</v>
       </c>
-      <c r="I5" s="1297" t="s">
+      <c r="I5" s="878" t="s">
         <v>185</v>
       </c>
-      <c r="J5" s="1306" t="s">
+      <c r="J5" s="887" t="s">
         <v>186</v>
       </c>
       <c r="K5"/>
-      <c r="L5" s="1315" t="s">
+      <c r="L5" s="896" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="84" x14ac:dyDescent="0.15">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="1253" t="s">
+      <c r="C6" s="834" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="1262" t="s">
+      <c r="D6" s="843" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="1271" t="s">
+      <c r="E6" s="852" t="s">
         <v>187</v>
       </c>
-      <c r="F6" s="1280" t="s">
+      <c r="F6" s="861" t="s">
         <v>188</v>
       </c>
       <c r="G6" s="90"/>
-      <c r="H6" s="1289" t="s">
+      <c r="H6" s="870" t="s">
         <v>189</v>
       </c>
-      <c r="I6" s="1298" t="s">
+      <c r="I6" s="879" t="s">
         <v>190</v>
       </c>
-      <c r="J6" s="1307" t="s">
+      <c r="J6" s="888" t="s">
         <v>191</v>
       </c>
       <c r="K6"/>
-      <c r="L6" s="1316" t="s">
+      <c r="L6" s="897" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="98" x14ac:dyDescent="0.15">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="1254" t="s">
+      <c r="C7" s="835" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="1263" t="s">
+      <c r="D7" s="844" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="1272" t="s">
+      <c r="E7" s="853" t="s">
         <v>192</v>
       </c>
-      <c r="F7" s="1281" t="s">
+      <c r="F7" s="862" t="s">
         <v>193</v>
       </c>
       <c r="G7" s="91"/>
-      <c r="H7" s="1290" t="s">
+      <c r="H7" s="871" t="s">
         <v>194</v>
       </c>
-      <c r="I7" s="1299" t="s">
+      <c r="I7" s="880" t="s">
         <v>195</v>
       </c>
-      <c r="J7" s="1308" t="s">
+      <c r="J7" s="889" t="s">
         <v>196</v>
       </c>
       <c r="K7"/>
-      <c r="L7" s="1317" t="s">
+      <c r="L7" s="898" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="84" x14ac:dyDescent="0.15">
       <c r="A8" s="19"/>
       <c r="B8"/>
-      <c r="C8" s="1255" t="s">
+      <c r="C8" s="836" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="1264" t="s">
+      <c r="D8" s="845" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="1273" t="s">
+      <c r="E8" s="854" t="s">
         <v>197</v>
       </c>
-      <c r="F8" s="1282" t="s">
+      <c r="F8" s="863" t="s">
         <v>198</v>
       </c>
       <c r="G8" s="92"/>
-      <c r="H8" s="1291" t="s">
+      <c r="H8" s="872" t="s">
         <v>199</v>
       </c>
-      <c r="I8" s="1300" t="s">
+      <c r="I8" s="881" t="s">
         <v>200</v>
       </c>
-      <c r="J8" s="1309" t="s">
+      <c r="J8" s="890" t="s">
         <v>201</v>
       </c>
       <c r="K8"/>
-      <c r="L8" s="1318" t="s">
+      <c r="L8" s="899" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="84" x14ac:dyDescent="0.15">
       <c r="A9" s="19"/>
       <c r="B9"/>
-      <c r="C9" s="1256" t="s">
+      <c r="C9" s="837" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="1265" t="s">
+      <c r="D9" s="846" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="1274" t="s">
+      <c r="E9" s="855" t="s">
         <v>202</v>
       </c>
-      <c r="F9" s="1283" t="s">
+      <c r="F9" s="864" t="s">
         <v>203</v>
       </c>
       <c r="G9" s="93"/>
-      <c r="H9" s="1292" t="s">
+      <c r="H9" s="873" t="s">
         <v>204</v>
       </c>
-      <c r="I9" s="1301" t="s">
+      <c r="I9" s="882" t="s">
         <v>205</v>
       </c>
-      <c r="J9" s="1310" t="s">
+      <c r="J9" s="891" t="s">
         <v>206</v>
       </c>
       <c r="K9"/>
-      <c r="L9" s="1319" t="s">
+      <c r="L9" s="900" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="84" x14ac:dyDescent="0.15">
       <c r="A10" s="19"/>
       <c r="B10"/>
-      <c r="C10" s="1257" t="s">
+      <c r="C10" s="838" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="1266" t="s">
+      <c r="D10" s="847" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="1275" t="s">
+      <c r="E10" s="856" t="s">
         <v>207</v>
       </c>
-      <c r="F10" s="1284" t="s">
+      <c r="F10" s="865" t="s">
         <v>208</v>
       </c>
       <c r="G10" s="94"/>
-      <c r="H10" s="1293" t="s">
+      <c r="H10" s="874" t="s">
         <v>209</v>
       </c>
-      <c r="I10" s="1302" t="s">
+      <c r="I10" s="883" t="s">
         <v>210</v>
       </c>
-      <c r="J10" s="1311" t="s">
+      <c r="J10" s="892" t="s">
         <v>211</v>
       </c>
       <c r="K10"/>
-      <c r="L10" s="1320" t="s">
+      <c r="L10" s="901" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="84" x14ac:dyDescent="0.15">
       <c r="A11" s="19"/>
       <c r="B11"/>
-      <c r="C11" s="1258" t="s">
+      <c r="C11" s="839" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="1267" t="s">
+      <c r="D11" s="848" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="1276" t="s">
+      <c r="E11" s="857" t="s">
         <v>212</v>
       </c>
-      <c r="F11" s="1285" t="s">
+      <c r="F11" s="866" t="s">
         <v>213</v>
       </c>
       <c r="G11" s="95"/>
-      <c r="H11" s="1294" t="s">
+      <c r="H11" s="875" t="s">
         <v>214</v>
       </c>
-      <c r="I11" s="1303" t="s">
+      <c r="I11" s="884" t="s">
         <v>215</v>
       </c>
-      <c r="J11" s="1312" t="s">
+      <c r="J11" s="893" t="s">
         <v>216</v>
       </c>
       <c r="K11"/>
-      <c r="L11" s="1321" t="s">
+      <c r="L11" s="902" t="s">
         <v>333</v>
       </c>
     </row>
@@ -17467,7 +16244,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17488,19 +16265,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="524" t="s">
+      <c r="A1" s="532" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="520"/>
-      <c r="C1" s="520"/>
-      <c r="D1" s="520"/>
-      <c r="E1" s="520"/>
-      <c r="F1" s="520"/>
-      <c r="G1" s="520"/>
-      <c r="H1" s="520"/>
-      <c r="I1" s="520"/>
-      <c r="J1" s="520"/>
-      <c r="K1" s="521"/>
+      <c r="B1" s="528"/>
+      <c r="C1" s="528"/>
+      <c r="D1" s="528"/>
+      <c r="E1" s="528"/>
+      <c r="F1" s="528"/>
+      <c r="G1" s="528"/>
+      <c r="H1" s="528"/>
+      <c r="I1" s="528"/>
+      <c r="J1" s="528"/>
+      <c r="K1" s="529"/>
     </row>
     <row r="2" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -17533,7 +16310,7 @@
       <c r="J2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="526" t="s">
+      <c r="K2" s="102" t="s">
         <v>218</v>
       </c>
       <c r="L2" s="9"/>
@@ -17560,32 +16337,32 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="1322" t="s">
+      <c r="C3" s="903" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1328" t="s">
+      <c r="D3" s="909" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="1334" t="s">
+      <c r="E3" s="915" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="1340" t="s">
+      <c r="F3" s="921" t="s">
         <v>219</v>
       </c>
-      <c r="G3" s="1346" t="s">
+      <c r="G3" s="927" t="s">
         <v>220</v>
       </c>
-      <c r="H3" s="1352" t="s">
+      <c r="H3" s="933" t="s">
         <v>334</v>
       </c>
       <c r="I3" s="96"/>
-      <c r="J3" s="1358" t="s">
+      <c r="J3" s="939" t="s">
         <v>370</v>
       </c>
-      <c r="K3" s="1364" t="s">
+      <c r="K3" s="945" t="s">
         <v>221</v>
       </c>
-      <c r="L3" s="1370" t="s">
+      <c r="L3" s="951" t="s">
         <v>340</v>
       </c>
       <c r="U3" s="6"/>
@@ -17601,32 +16378,32 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="1323" t="s">
+      <c r="C4" s="904" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="1329" t="s">
+      <c r="D4" s="910" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="1335" t="s">
+      <c r="E4" s="916" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="1341" t="s">
+      <c r="F4" s="922" t="s">
         <v>376</v>
       </c>
-      <c r="G4" s="1347" t="s">
+      <c r="G4" s="928" t="s">
         <v>367</v>
       </c>
-      <c r="H4" s="1353" t="s">
+      <c r="H4" s="934" t="s">
         <v>335</v>
       </c>
       <c r="I4" s="97"/>
-      <c r="J4" s="1359" t="s">
+      <c r="J4" s="940" t="s">
         <v>371</v>
       </c>
-      <c r="K4" s="1365" t="s">
+      <c r="K4" s="946" t="s">
         <v>377</v>
       </c>
-      <c r="L4" s="1371" t="s">
+      <c r="L4" s="952" t="s">
         <v>341</v>
       </c>
       <c r="U4" s="6"/>
@@ -17642,32 +16419,32 @@
     <row r="5" spans="1:31" ht="128" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="1324" t="s">
+      <c r="C5" s="905" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="1330" t="s">
+      <c r="D5" s="911" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="1336" t="s">
+      <c r="E5" s="917" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="1342" t="s">
+      <c r="F5" s="923" t="s">
         <v>219</v>
       </c>
-      <c r="G5" s="1348" t="s">
+      <c r="G5" s="929" t="s">
         <v>222</v>
       </c>
-      <c r="H5" s="1354" t="s">
+      <c r="H5" s="935" t="s">
         <v>336</v>
       </c>
       <c r="I5" s="98"/>
-      <c r="J5" s="1360" t="s">
+      <c r="J5" s="941" t="s">
         <v>372</v>
       </c>
-      <c r="K5" s="1366" t="s">
+      <c r="K5" s="947" t="s">
         <v>221</v>
       </c>
-      <c r="L5" s="1372" t="s">
+      <c r="L5" s="953" t="s">
         <v>342</v>
       </c>
       <c r="U5" s="6"/>
@@ -17683,32 +16460,32 @@
     <row r="6" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="1325" t="s">
+      <c r="C6" s="906" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="1331" t="s">
+      <c r="D6" s="912" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="1337" t="s">
+      <c r="E6" s="918" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="1343" t="s">
+      <c r="F6" s="924" t="s">
         <v>376</v>
       </c>
-      <c r="G6" s="1349" t="s">
+      <c r="G6" s="930" t="s">
         <v>368</v>
       </c>
-      <c r="H6" s="1355" t="s">
+      <c r="H6" s="936" t="s">
         <v>337</v>
       </c>
       <c r="I6" s="99"/>
-      <c r="J6" s="1361" t="s">
+      <c r="J6" s="942" t="s">
         <v>373</v>
       </c>
-      <c r="K6" s="1367" t="s">
+      <c r="K6" s="948" t="s">
         <v>377</v>
       </c>
-      <c r="L6" s="1373" t="s">
+      <c r="L6" s="954" t="s">
         <v>343</v>
       </c>
       <c r="U6" s="6"/>
@@ -17724,32 +16501,32 @@
     <row r="7" spans="1:31" ht="128" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="1326" t="s">
+      <c r="C7" s="907" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="1332" t="s">
+      <c r="D7" s="913" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="1338" t="s">
+      <c r="E7" s="919" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="1344" t="s">
+      <c r="F7" s="925" t="s">
         <v>219</v>
       </c>
-      <c r="G7" s="1350" t="s">
+      <c r="G7" s="931" t="s">
         <v>223</v>
       </c>
-      <c r="H7" s="1356" t="s">
+      <c r="H7" s="937" t="s">
         <v>338</v>
       </c>
       <c r="I7" s="100"/>
-      <c r="J7" s="1362" t="s">
+      <c r="J7" s="943" t="s">
         <v>374</v>
       </c>
-      <c r="K7" s="1368" t="s">
+      <c r="K7" s="949" t="s">
         <v>224</v>
       </c>
-      <c r="L7" s="1374" t="s">
+      <c r="L7" s="955" t="s">
         <v>344</v>
       </c>
       <c r="U7" s="6"/>
@@ -17765,32 +16542,32 @@
     <row r="8" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8"/>
-      <c r="C8" s="1327" t="s">
+      <c r="C8" s="908" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="1333" t="s">
+      <c r="D8" s="914" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="1339" t="s">
+      <c r="E8" s="920" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="1345" t="s">
+      <c r="F8" s="926" t="s">
         <v>376</v>
       </c>
-      <c r="G8" s="1351" t="s">
+      <c r="G8" s="932" t="s">
         <v>369</v>
       </c>
-      <c r="H8" s="1357" t="s">
+      <c r="H8" s="938" t="s">
         <v>339</v>
       </c>
       <c r="I8" s="101"/>
-      <c r="J8" s="1363" t="s">
+      <c r="J8" s="944" t="s">
         <v>375</v>
       </c>
-      <c r="K8" s="1369" t="s">
+      <c r="K8" s="950" t="s">
         <v>377</v>
       </c>
-      <c r="L8" s="1375" t="s">
+      <c r="L8" s="956" t="s">
         <v>345</v>
       </c>
       <c r="U8" s="6"/>
@@ -17806,7 +16583,7 @@
     <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="E9" s="19"/>
-      <c r="K9" s="528"/>
+      <c r="K9" s="103"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -17820,7 +16597,7 @@
     <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="E10" s="19"/>
-      <c r="K10" s="528"/>
+      <c r="K10" s="103"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
@@ -17834,7 +16611,7 @@
     <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="E11" s="19"/>
-      <c r="K11" s="528"/>
+      <c r="K11" s="103"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
@@ -17848,7 +16625,7 @@
     <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="E12" s="19"/>
-      <c r="K12" s="528"/>
+      <c r="K12" s="103"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
@@ -17862,7 +16639,7 @@
     <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="E13" s="19"/>
-      <c r="K13" s="528"/>
+      <c r="K13" s="103"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
@@ -17876,7 +16653,7 @@
     <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="E14" s="19"/>
-      <c r="K14" s="528"/>
+      <c r="K14" s="103"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
@@ -17890,7 +16667,7 @@
     <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="E15" s="19"/>
-      <c r="K15" s="528"/>
+      <c r="K15" s="103"/>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
@@ -17904,7 +16681,7 @@
     <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="E16" s="19"/>
-      <c r="K16" s="528"/>
+      <c r="K16" s="103"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
@@ -17918,7 +16695,7 @@
     <row r="17" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="E17" s="19"/>
-      <c r="K17" s="528"/>
+      <c r="K17" s="103"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
@@ -17932,7 +16709,7 @@
     <row r="18" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="E18" s="19"/>
-      <c r="K18" s="528"/>
+      <c r="K18" s="103"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
@@ -17946,7 +16723,7 @@
     <row r="19" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="E19" s="19"/>
-      <c r="K19" s="528"/>
+      <c r="K19" s="103"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
@@ -17960,7 +16737,7 @@
     <row r="20" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="E20" s="19"/>
-      <c r="K20" s="528"/>
+      <c r="K20" s="103"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
@@ -17974,7 +16751,7 @@
     <row r="21" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="E21" s="19"/>
-      <c r="K21" s="528"/>
+      <c r="K21" s="103"/>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
@@ -17988,7 +16765,7 @@
     <row r="22" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="E22" s="19"/>
-      <c r="K22" s="528"/>
+      <c r="K22" s="103"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
@@ -18002,7 +16779,7 @@
     <row r="23" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="E23" s="19"/>
-      <c r="K23" s="528"/>
+      <c r="K23" s="103"/>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
@@ -18016,7 +16793,7 @@
     <row r="24" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="E24" s="19"/>
-      <c r="K24" s="528"/>
+      <c r="K24" s="103"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
@@ -18030,7 +16807,7 @@
     <row r="25" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="E25" s="19"/>
-      <c r="K25" s="528"/>
+      <c r="K25" s="103"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
@@ -18044,7 +16821,7 @@
     <row r="26" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="E26" s="19"/>
-      <c r="K26" s="528"/>
+      <c r="K26" s="103"/>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
@@ -18058,7 +16835,7 @@
     <row r="27" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="E27" s="19"/>
-      <c r="K27" s="528"/>
+      <c r="K27" s="103"/>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
@@ -18072,7 +16849,7 @@
     <row r="28" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="E28" s="19"/>
-      <c r="K28" s="528"/>
+      <c r="K28" s="103"/>
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
@@ -18086,7 +16863,7 @@
     <row r="29" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="E29" s="19"/>
-      <c r="K29" s="528"/>
+      <c r="K29" s="103"/>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
       <c r="W29" s="6"/>
@@ -18100,7 +16877,7 @@
     <row r="30" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="E30" s="19"/>
-      <c r="K30" s="528"/>
+      <c r="K30" s="103"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
@@ -18114,7 +16891,7 @@
     <row r="31" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="E31" s="19"/>
-      <c r="K31" s="528"/>
+      <c r="K31" s="103"/>
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
       <c r="W31" s="6"/>
@@ -18128,7 +16905,7 @@
     <row r="32" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="E32" s="19"/>
-      <c r="K32" s="528"/>
+      <c r="K32" s="103"/>
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
       <c r="W32" s="6"/>
@@ -18142,7 +16919,7 @@
     <row r="33" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="E33" s="19"/>
-      <c r="K33" s="528"/>
+      <c r="K33" s="103"/>
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
       <c r="W33" s="6"/>
@@ -18156,7 +16933,7 @@
     <row r="34" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="E34" s="19"/>
-      <c r="K34" s="528"/>
+      <c r="K34" s="103"/>
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
       <c r="W34" s="6"/>
@@ -18170,7 +16947,7 @@
     <row r="35" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="E35" s="19"/>
-      <c r="K35" s="528"/>
+      <c r="K35" s="103"/>
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
       <c r="W35" s="6"/>
@@ -18184,7 +16961,7 @@
     <row r="36" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="E36" s="19"/>
-      <c r="K36" s="528"/>
+      <c r="K36" s="103"/>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
       <c r="W36" s="6"/>
@@ -19078,22 +17855,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="525" t="s">
+      <c r="A1" s="533" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="520"/>
-      <c r="C1" s="520"/>
-      <c r="D1" s="520"/>
-      <c r="E1" s="520"/>
-      <c r="F1" s="520"/>
-      <c r="G1" s="520"/>
-      <c r="H1" s="520"/>
-      <c r="I1" s="520"/>
-      <c r="J1" s="520"/>
-      <c r="K1" s="520"/>
-      <c r="L1" s="520"/>
-      <c r="M1" s="520"/>
-      <c r="N1" s="521"/>
+      <c r="B1" s="528"/>
+      <c r="C1" s="528"/>
+      <c r="D1" s="528"/>
+      <c r="E1" s="528"/>
+      <c r="F1" s="528"/>
+      <c r="G1" s="528"/>
+      <c r="H1" s="528"/>
+      <c r="I1" s="528"/>
+      <c r="J1" s="528"/>
+      <c r="K1" s="528"/>
+      <c r="L1" s="528"/>
+      <c r="M1" s="528"/>
+      <c r="N1" s="529"/>
     </row>
     <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">

</xml_diff>